<commit_message>
Update for Dec 3
</commit_message>
<xml_diff>
--- a/data/CasesByDate.xlsx
+++ b/data/CasesByDate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\COVID-19 Data Visualization\COVID19 - Files\Power BI resources\CSV filesPROB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEAB5BB-FA16-4EC9-8E8E-2BA56FA65C18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9751C0-1F32-418F-A0BA-73B2B5FD2557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,13 +884,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D309"/>
+  <dimension ref="A1:D310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B287" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:C309"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2:C310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5120,14 +5120,14 @@
       </c>
       <c r="B266">
         <f t="shared" si="8"/>
-        <v>143825</v>
+        <v>143826</v>
       </c>
       <c r="C266">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="D266">
         <f t="shared" ref="D266:D279" si="9">AVERAGE(C260:C266)</f>
-        <v>779.57142857142856</v>
+        <v>779.71428571428567</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.35">
@@ -5136,14 +5136,14 @@
       </c>
       <c r="B267">
         <f t="shared" si="8"/>
-        <v>144945</v>
+        <v>144946</v>
       </c>
       <c r="C267">
         <v>1120</v>
       </c>
       <c r="D267">
         <f t="shared" si="9"/>
-        <v>827</v>
+        <v>827.14285714285711</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.35">
@@ -5152,14 +5152,14 @@
       </c>
       <c r="B268">
         <f t="shared" si="8"/>
-        <v>146148</v>
+        <v>146149</v>
       </c>
       <c r="C268">
         <v>1203</v>
       </c>
       <c r="D268">
         <f t="shared" si="9"/>
-        <v>870.42857142857144</v>
+        <v>870.57142857142856</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.35">
@@ -5168,14 +5168,14 @@
       </c>
       <c r="B269">
         <f t="shared" si="8"/>
-        <v>147527</v>
+        <v>147528</v>
       </c>
       <c r="C269">
         <v>1379</v>
       </c>
       <c r="D269">
         <f t="shared" si="9"/>
-        <v>931.57142857142856</v>
+        <v>931.71428571428567</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.35">
@@ -5187,7 +5187,7 @@
         <v>148754</v>
       </c>
       <c r="C270">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D270">
         <f t="shared" si="9"/>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="D273">
         <f t="shared" si="9"/>
-        <v>1103.5714285714287</v>
+        <v>1103.4285714285713</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.35">
@@ -5255,7 +5255,7 @@
       </c>
       <c r="D274">
         <f t="shared" si="9"/>
-        <v>1135.8571428571429</v>
+        <v>1135.7142857142858</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.35">
@@ -5264,10 +5264,10 @@
       </c>
       <c r="B275">
         <f t="shared" si="8"/>
-        <v>154338</v>
+        <v>154339</v>
       </c>
       <c r="C275">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D275">
         <f t="shared" si="9"/>
@@ -5283,11 +5283,11 @@
         <v>155725</v>
       </c>
       <c r="C276">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="D276">
         <f t="shared" si="9"/>
-        <v>1171.1428571428571</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.35">
@@ -5350,7 +5350,7 @@
         <v>1839</v>
       </c>
       <c r="D280">
-        <f t="shared" ref="D280:D309" si="10">AVERAGE(C274:C280)</f>
+        <f t="shared" ref="D280:D310" si="10">AVERAGE(C274:C280)</f>
         <v>1219</v>
       </c>
     </row>
@@ -5383,7 +5383,7 @@
       </c>
       <c r="D282">
         <f t="shared" si="10"/>
-        <v>1404.8571428571429</v>
+        <v>1404.7142857142858</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.35">
@@ -5392,14 +5392,14 @@
       </c>
       <c r="B283">
         <f t="shared" si="8"/>
-        <v>166587</v>
+        <v>166589</v>
       </c>
       <c r="C283">
-        <v>2415</v>
+        <v>2417</v>
       </c>
       <c r="D283">
         <f t="shared" si="10"/>
-        <v>1551.7142857142858</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.35">
@@ -5408,14 +5408,14 @@
       </c>
       <c r="B284">
         <f t="shared" si="8"/>
-        <v>168825</v>
+        <v>168827</v>
       </c>
       <c r="C284">
         <v>2238</v>
       </c>
       <c r="D284">
         <f t="shared" si="10"/>
-        <v>1710.7142857142858</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.35">
@@ -5424,14 +5424,14 @@
       </c>
       <c r="B285">
         <f t="shared" si="8"/>
-        <v>170151</v>
+        <v>170153</v>
       </c>
       <c r="C285">
         <v>1326</v>
       </c>
       <c r="D285">
         <f t="shared" si="10"/>
-        <v>1775.5714285714287</v>
+        <v>1775.8571428571429</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.35">
@@ -5440,14 +5440,14 @@
       </c>
       <c r="B286">
         <f t="shared" si="8"/>
-        <v>171094</v>
+        <v>171096</v>
       </c>
       <c r="C286">
         <v>943</v>
       </c>
       <c r="D286">
         <f t="shared" si="10"/>
-        <v>1835.7142857142858</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.35">
@@ -5455,15 +5455,15 @@
         <v>44144</v>
       </c>
       <c r="B287">
-        <f t="shared" ref="B287:B309" si="11">C287+B286</f>
-        <v>174273</v>
+        <f t="shared" ref="B287:B310" si="11">C287+B286</f>
+        <v>174275</v>
       </c>
       <c r="C287">
         <v>3179</v>
       </c>
       <c r="D287">
         <f t="shared" si="10"/>
-        <v>2027.1428571428571</v>
+        <v>2027.4285714285713</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.35">
@@ -5472,14 +5472,14 @@
       </c>
       <c r="B288">
         <f t="shared" si="11"/>
-        <v>177096</v>
+        <v>177099</v>
       </c>
       <c r="C288">
-        <v>2823</v>
+        <v>2824</v>
       </c>
       <c r="D288">
         <f t="shared" si="10"/>
-        <v>2157.4285714285716</v>
+        <v>2157.8571428571427</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.35">
@@ -5488,14 +5488,14 @@
       </c>
       <c r="B289">
         <f t="shared" si="11"/>
-        <v>179762</v>
+        <v>179765</v>
       </c>
       <c r="C289">
         <v>2666</v>
       </c>
       <c r="D289">
         <f t="shared" si="10"/>
-        <v>2227.1428571428573</v>
+        <v>2227.5714285714284</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.35">
@@ -5504,14 +5504,14 @@
       </c>
       <c r="B290">
         <f t="shared" si="11"/>
-        <v>182752</v>
+        <v>182758</v>
       </c>
       <c r="C290">
-        <v>2990</v>
+        <v>2993</v>
       </c>
       <c r="D290">
         <f t="shared" si="10"/>
-        <v>2309.2857142857142</v>
+        <v>2309.8571428571427</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.35">
@@ -5520,14 +5520,14 @@
       </c>
       <c r="B291">
         <f t="shared" si="11"/>
-        <v>185360</v>
+        <v>185367</v>
       </c>
       <c r="C291">
-        <v>2608</v>
+        <v>2609</v>
       </c>
       <c r="D291">
         <f t="shared" si="10"/>
-        <v>2362.1428571428573</v>
+        <v>2362.8571428571427</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.35">
@@ -5536,14 +5536,14 @@
       </c>
       <c r="B292">
         <f t="shared" si="11"/>
-        <v>187075</v>
+        <v>187082</v>
       </c>
       <c r="C292">
         <v>1715</v>
       </c>
       <c r="D292">
         <f t="shared" si="10"/>
-        <v>2417.7142857142858</v>
+        <v>2418.4285714285716</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.35">
@@ -5552,14 +5552,14 @@
       </c>
       <c r="B293">
         <f t="shared" si="11"/>
-        <v>188270</v>
+        <v>188277</v>
       </c>
       <c r="C293">
         <v>1195</v>
       </c>
       <c r="D293">
         <f t="shared" si="10"/>
-        <v>2453.7142857142858</v>
+        <v>2454.4285714285716</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.35">
@@ -5568,14 +5568,14 @@
       </c>
       <c r="B294">
         <f t="shared" si="11"/>
-        <v>191791</v>
+        <v>191798</v>
       </c>
       <c r="C294">
         <v>3521</v>
       </c>
       <c r="D294">
         <f>AVERAGE(C288:C294)</f>
-        <v>2502.5714285714284</v>
+        <v>2503.2857142857142</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.35">
@@ -5584,14 +5584,14 @@
       </c>
       <c r="B295">
         <f t="shared" si="11"/>
-        <v>194920</v>
+        <v>194935</v>
       </c>
       <c r="C295">
-        <v>3129</v>
+        <v>3137</v>
       </c>
       <c r="D295">
         <f t="shared" si="10"/>
-        <v>2546.2857142857142</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.35">
@@ -5600,14 +5600,14 @@
       </c>
       <c r="B296">
         <f t="shared" si="11"/>
-        <v>197841</v>
+        <v>197856</v>
       </c>
       <c r="C296">
         <v>2921</v>
       </c>
       <c r="D296">
         <f t="shared" si="10"/>
-        <v>2582.7142857142858</v>
+        <v>2584.4285714285716</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.35">
@@ -5616,14 +5616,14 @@
       </c>
       <c r="B297">
         <f t="shared" si="11"/>
-        <v>200842</v>
+        <v>200858</v>
       </c>
       <c r="C297">
-        <v>3001</v>
+        <v>3002</v>
       </c>
       <c r="D297">
         <f t="shared" si="10"/>
-        <v>2584.2857142857142</v>
+        <v>2585.7142857142858</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.35">
@@ -5632,14 +5632,14 @@
       </c>
       <c r="B298">
         <f t="shared" si="11"/>
-        <v>203703</v>
+        <v>203721</v>
       </c>
       <c r="C298">
-        <v>2861</v>
+        <v>2863</v>
       </c>
       <c r="D298">
         <f t="shared" si="10"/>
-        <v>2620.4285714285716</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.35">
@@ -5648,14 +5648,14 @@
       </c>
       <c r="B299">
         <f t="shared" si="11"/>
-        <v>205470</v>
+        <v>205493</v>
       </c>
       <c r="C299">
-        <v>1767</v>
+        <v>1772</v>
       </c>
       <c r="D299">
         <f t="shared" si="10"/>
-        <v>2627.8571428571427</v>
+        <v>2630.1428571428573</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.35">
@@ -5664,14 +5664,14 @@
       </c>
       <c r="B300">
         <f t="shared" si="11"/>
-        <v>206654</v>
+        <v>206681</v>
       </c>
       <c r="C300">
-        <v>1184</v>
+        <v>1188</v>
       </c>
       <c r="D300">
         <f t="shared" si="10"/>
-        <v>2626.2857142857142</v>
+        <v>2629.1428571428573</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.35">
@@ -5680,14 +5680,14 @@
       </c>
       <c r="B301">
         <f t="shared" si="11"/>
-        <v>210127</v>
+        <v>210266</v>
       </c>
       <c r="C301">
-        <v>3473</v>
+        <v>3585</v>
       </c>
       <c r="D301">
         <f t="shared" si="10"/>
-        <v>2619.4285714285716</v>
+        <v>2638.2857142857142</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.35">
@@ -5696,14 +5696,14 @@
       </c>
       <c r="B302">
         <f t="shared" si="11"/>
-        <v>213697</v>
+        <v>214046</v>
       </c>
       <c r="C302">
-        <v>3570</v>
+        <v>3780</v>
       </c>
       <c r="D302">
         <f t="shared" si="10"/>
-        <v>2682.4285714285716</v>
+        <v>2730.1428571428573</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.35">
@@ -5712,14 +5712,14 @@
       </c>
       <c r="B303">
         <f t="shared" si="11"/>
-        <v>216437</v>
+        <v>216977</v>
       </c>
       <c r="C303">
-        <v>2740</v>
+        <v>2931</v>
       </c>
       <c r="D303">
         <f t="shared" si="10"/>
-        <v>2656.5714285714284</v>
+        <v>2731.5714285714284</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.35">
@@ -5728,14 +5728,14 @@
       </c>
       <c r="B304">
         <f t="shared" si="11"/>
-        <v>216845</v>
+        <v>217407</v>
       </c>
       <c r="C304">
-        <v>408</v>
+        <v>430</v>
       </c>
       <c r="D304">
         <f t="shared" si="10"/>
-        <v>2286.1428571428573</v>
+        <v>2364.1428571428573</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.35">
@@ -5744,14 +5744,14 @@
       </c>
       <c r="B305">
         <f t="shared" si="11"/>
-        <v>219701</v>
+        <v>220627</v>
       </c>
       <c r="C305">
-        <v>2856</v>
+        <v>3220</v>
       </c>
       <c r="D305">
         <f t="shared" si="10"/>
-        <v>2285.4285714285716</v>
+        <v>2415.1428571428573</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.35">
@@ -5760,14 +5760,14 @@
       </c>
       <c r="B306">
         <f t="shared" si="11"/>
-        <v>221868</v>
+        <v>223333</v>
       </c>
       <c r="C306">
-        <v>2167</v>
+        <v>2706</v>
       </c>
       <c r="D306">
         <f t="shared" si="10"/>
-        <v>2342.5714285714284</v>
+        <v>2548.5714285714284</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.35">
@@ -5776,14 +5776,14 @@
       </c>
       <c r="B307">
         <f t="shared" si="11"/>
-        <v>222974</v>
+        <v>224763</v>
       </c>
       <c r="C307">
-        <v>1106</v>
+        <v>1430</v>
       </c>
       <c r="D307">
         <f t="shared" si="10"/>
-        <v>2331.4285714285716</v>
+        <v>2583.1428571428573</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.35">
@@ -5792,14 +5792,14 @@
       </c>
       <c r="B308">
         <f t="shared" si="11"/>
-        <v>225533</v>
+        <v>228567</v>
       </c>
       <c r="C308">
-        <v>2559</v>
+        <v>3804</v>
       </c>
       <c r="D308">
         <f t="shared" si="10"/>
-        <v>2200.8571428571427</v>
+        <v>2614.4285714285716</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.35">
@@ -5808,14 +5808,30 @@
       </c>
       <c r="B309">
         <f t="shared" si="11"/>
-        <v>225787</v>
+        <v>231857</v>
       </c>
       <c r="C309">
-        <v>254</v>
+        <v>3290</v>
       </c>
       <c r="D309">
         <f t="shared" si="10"/>
-        <v>1727.1428571428571</v>
+        <v>2544.4285714285716</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A310" s="1">
+        <v>44167</v>
+      </c>
+      <c r="B310">
+        <f t="shared" si="11"/>
+        <v>232264</v>
+      </c>
+      <c r="C310">
+        <v>407</v>
+      </c>
+      <c r="D310">
+        <f t="shared" si="10"/>
+        <v>2183.8571428571427</v>
       </c>
     </row>
   </sheetData>
@@ -5824,15 +5840,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008004546134034441816F24C41F65E929" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c3392cbe151f976ef883c2eee1f53348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0967b7be50301903c78f9c39c6fd9af8">
     <xsd:element name="properties">
@@ -5946,21 +5953,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C76A581D-70D9-4324-B3C2-C549CBC3A500}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A7812BB-980B-4585-92C6-973734300155}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5976,11 +5984,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E2A907-BC75-4262-BBD0-4F1B2976CD82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C76A581D-70D9-4324-B3C2-C549CBC3A500}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update for yesterday. Added weekly graphs and source file
</commit_message>
<xml_diff>
--- a/data/CasesByDate.xlsx
+++ b/data/CasesByDate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\COVID-19 Data Visualization\COVID19 - Files\Power BI resources\CSV filesPROB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA01A555-8D6A-4D85-9518-889AC2477900}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D528E218-B7FC-4B5D-B142-D63EA21C7BC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -881,13 +881,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D312"/>
+  <dimension ref="A1:D313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B295" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B299" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J309" sqref="J309"/>
+      <selection pane="bottomRight" activeCell="E316" sqref="E316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,14 +2125,14 @@
       </c>
       <c r="B79">
         <f t="shared" si="2"/>
-        <v>35724</v>
+        <v>35723</v>
       </c>
       <c r="C79">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="D79">
         <f t="shared" si="3"/>
-        <v>1963.7142857142858</v>
+        <v>1963.5714285714287</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2141,14 +2141,14 @@
       </c>
       <c r="B80">
         <f t="shared" si="2"/>
-        <v>38110</v>
+        <v>38109</v>
       </c>
       <c r="C80">
         <v>2386</v>
       </c>
       <c r="D80">
         <f t="shared" si="3"/>
-        <v>2022</v>
+        <v>2021.8571428571429</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2157,14 +2157,14 @@
       </c>
       <c r="B81">
         <f t="shared" si="2"/>
-        <v>41100</v>
+        <v>41099</v>
       </c>
       <c r="C81">
         <v>2990</v>
       </c>
       <c r="D81">
         <f t="shared" si="3"/>
-        <v>2155.5714285714284</v>
+        <v>2155.4285714285716</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2173,14 +2173,14 @@
       </c>
       <c r="B82">
         <f t="shared" si="2"/>
-        <v>42581</v>
+        <v>42580</v>
       </c>
       <c r="C82">
         <v>1481</v>
       </c>
       <c r="D82">
         <f t="shared" si="3"/>
-        <v>2177.2857142857142</v>
+        <v>2177.1428571428573</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2189,14 +2189,14 @@
       </c>
       <c r="B83">
         <f t="shared" si="2"/>
-        <v>43670</v>
+        <v>43669</v>
       </c>
       <c r="C83">
         <v>1089</v>
       </c>
       <c r="D83">
         <f t="shared" si="3"/>
-        <v>2200</v>
+        <v>2199.8571428571427</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2205,14 +2205,14 @@
       </c>
       <c r="B84">
         <f t="shared" si="2"/>
-        <v>46356</v>
+        <v>46355</v>
       </c>
       <c r="C84">
         <v>2686</v>
       </c>
       <c r="D84">
         <f t="shared" si="3"/>
-        <v>2300</v>
+        <v>2299.8571428571427</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2221,14 +2221,14 @@
       </c>
       <c r="B85">
         <f t="shared" si="2"/>
-        <v>48543</v>
+        <v>48542</v>
       </c>
       <c r="C85">
         <v>2187</v>
       </c>
       <c r="D85">
         <f t="shared" si="3"/>
-        <v>2194.2857142857142</v>
+        <v>2194.1428571428573</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>51247</v>
+        <v>51246</v>
       </c>
       <c r="C86">
         <v>2704</v>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>53652</v>
+        <v>53651</v>
       </c>
       <c r="C87">
         <v>2405</v>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>55929</v>
+        <v>55928</v>
       </c>
       <c r="C88">
         <v>2277</v>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>57423</v>
+        <v>57422</v>
       </c>
       <c r="C89">
         <v>1494</v>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>58267</v>
+        <v>58266</v>
       </c>
       <c r="C90">
         <v>844</v>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>60396</v>
+        <v>60395</v>
       </c>
       <c r="C91">
         <v>2129</v>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>62500</v>
+        <v>62499</v>
       </c>
       <c r="C92">
         <v>2104</v>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>64686</v>
+        <v>64685</v>
       </c>
       <c r="C93">
         <v>2186</v>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>66733</v>
+        <v>66732</v>
       </c>
       <c r="C94">
         <v>2047</v>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>68814</v>
+        <v>68813</v>
       </c>
       <c r="C95">
         <v>2081</v>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>69843</v>
+        <v>69842</v>
       </c>
       <c r="C96">
         <v>1029</v>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>70577</v>
+        <v>70576</v>
       </c>
       <c r="C97">
         <v>734</v>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>72456</v>
+        <v>72455</v>
       </c>
       <c r="C98">
         <v>1879</v>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>74191</v>
+        <v>74190</v>
       </c>
       <c r="C99">
         <v>1735</v>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>75890</v>
+        <v>75889</v>
       </c>
       <c r="C100">
         <v>1699</v>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>77567</v>
+        <v>77566</v>
       </c>
       <c r="C101">
         <v>1677</v>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>79021</v>
+        <v>79020</v>
       </c>
       <c r="C102">
         <v>1454</v>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>79704</v>
+        <v>79703</v>
       </c>
       <c r="C103">
         <v>683</v>
@@ -2525,7 +2525,7 @@
       </c>
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>80089</v>
+        <v>80088</v>
       </c>
       <c r="C104">
         <v>385</v>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>81395</v>
+        <v>81394</v>
       </c>
       <c r="C105">
         <v>1306</v>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>82845</v>
+        <v>82844</v>
       </c>
       <c r="C106">
         <v>1450</v>
@@ -2573,14 +2573,14 @@
       </c>
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>84159</v>
+        <v>84157</v>
       </c>
       <c r="C107">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="D107">
         <f t="shared" si="3"/>
-        <v>1181.2857142857142</v>
+        <v>1181.1428571428571</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2589,14 +2589,14 @@
       </c>
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>85474</v>
+        <v>85472</v>
       </c>
       <c r="C108">
         <v>1315</v>
       </c>
       <c r="D108">
         <f t="shared" si="3"/>
-        <v>1129.5714285714287</v>
+        <v>1129.4285714285713</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>86579</v>
+        <v>86577</v>
       </c>
       <c r="C109">
         <v>1105</v>
       </c>
       <c r="D109">
         <f t="shared" si="3"/>
-        <v>1079.7142857142858</v>
+        <v>1079.5714285714287</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2621,14 +2621,14 @@
       </c>
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>87224</v>
+        <v>87222</v>
       </c>
       <c r="C110">
         <v>645</v>
       </c>
       <c r="D110">
         <f t="shared" si="3"/>
-        <v>1074.2857142857142</v>
+        <v>1074.1428571428571</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2637,14 +2637,14 @@
       </c>
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>87587</v>
+        <v>87585</v>
       </c>
       <c r="C111">
         <v>363</v>
       </c>
       <c r="D111">
         <f t="shared" si="3"/>
-        <v>1071.1428571428571</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2653,14 +2653,14 @@
       </c>
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>88901</v>
+        <v>88899</v>
       </c>
       <c r="C112">
         <v>1314</v>
       </c>
       <c r="D112">
         <f t="shared" si="3"/>
-        <v>1072.2857142857142</v>
+        <v>1072.1428571428571</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2669,14 +2669,14 @@
       </c>
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>89974</v>
+        <v>89972</v>
       </c>
       <c r="C113">
         <v>1073</v>
       </c>
       <c r="D113">
         <f t="shared" si="3"/>
-        <v>1018.4285714285714</v>
+        <v>1018.2857142857143</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>90985</v>
+        <v>90983</v>
       </c>
       <c r="C114">
         <v>1011</v>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>91950</v>
+        <v>91948</v>
       </c>
       <c r="C115">
         <v>965</v>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>92813</v>
+        <v>92811</v>
       </c>
       <c r="C116">
         <v>863</v>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>93201</v>
+        <v>93199</v>
       </c>
       <c r="C117">
         <v>388</v>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>93503</v>
+        <v>93501</v>
       </c>
       <c r="C118">
         <v>302</v>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>93701</v>
+        <v>93699</v>
       </c>
       <c r="C119">
         <v>198</v>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>94565</v>
+        <v>94563</v>
       </c>
       <c r="C120">
         <v>864</v>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B121">
         <f t="shared" si="2"/>
-        <v>95252</v>
+        <v>95250</v>
       </c>
       <c r="C121">
         <v>687</v>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="B122">
         <f t="shared" si="2"/>
-        <v>95891</v>
+        <v>95889</v>
       </c>
       <c r="C122">
         <v>639</v>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="B123">
         <f t="shared" si="2"/>
-        <v>96421</v>
+        <v>96419</v>
       </c>
       <c r="C123">
         <v>530</v>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="B124">
         <f t="shared" si="2"/>
-        <v>96692</v>
+        <v>96690</v>
       </c>
       <c r="C124">
         <v>271</v>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="B125">
         <f t="shared" si="2"/>
-        <v>96853</v>
+        <v>96851</v>
       </c>
       <c r="C125">
         <v>161</v>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B126">
         <f t="shared" si="2"/>
-        <v>97361</v>
+        <v>97359</v>
       </c>
       <c r="C126">
         <v>508</v>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="B127">
         <f t="shared" si="2"/>
-        <v>97808</v>
+        <v>97806</v>
       </c>
       <c r="C127">
         <v>447</v>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="B128">
         <f t="shared" si="2"/>
-        <v>98267</v>
+        <v>98265</v>
       </c>
       <c r="C128">
         <v>459</v>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="B129">
         <f t="shared" si="2"/>
-        <v>98646</v>
+        <v>98644</v>
       </c>
       <c r="C129">
         <v>379</v>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="B130">
         <f t="shared" si="2"/>
-        <v>98983</v>
+        <v>98981</v>
       </c>
       <c r="C130">
         <v>337</v>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B131">
         <f t="shared" si="2"/>
-        <v>99131</v>
+        <v>99129</v>
       </c>
       <c r="C131">
         <v>148</v>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="B132">
         <f t="shared" ref="B132:B195" si="4">C132+B131</f>
-        <v>99282</v>
+        <v>99280</v>
       </c>
       <c r="C132">
         <v>151</v>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="B133">
         <f t="shared" si="4"/>
-        <v>99635</v>
+        <v>99633</v>
       </c>
       <c r="C133">
         <v>353</v>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="B134">
         <f t="shared" si="4"/>
-        <v>99978</v>
+        <v>99976</v>
       </c>
       <c r="C134">
         <v>343</v>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="B135">
         <f t="shared" si="4"/>
-        <v>100237</v>
+        <v>100235</v>
       </c>
       <c r="C135">
         <v>259</v>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B136">
         <f t="shared" si="4"/>
-        <v>100463</v>
+        <v>100461</v>
       </c>
       <c r="C136">
         <v>226</v>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="B137">
         <f t="shared" si="4"/>
-        <v>100717</v>
+        <v>100715</v>
       </c>
       <c r="C137">
         <v>254</v>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="B138">
         <f t="shared" si="4"/>
-        <v>100814</v>
+        <v>100812</v>
       </c>
       <c r="C138">
         <v>97</v>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="B139">
         <f t="shared" si="4"/>
-        <v>100890</v>
+        <v>100888</v>
       </c>
       <c r="C139">
         <v>76</v>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="B140">
         <f t="shared" si="4"/>
-        <v>101125</v>
+        <v>101123</v>
       </c>
       <c r="C140">
         <v>235</v>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B141">
         <f t="shared" si="4"/>
-        <v>101323</v>
+        <v>101321</v>
       </c>
       <c r="C141">
         <v>198</v>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="B142">
         <f t="shared" si="4"/>
-        <v>101572</v>
+        <v>101570</v>
       </c>
       <c r="C142">
         <v>249</v>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="B143">
         <f t="shared" si="4"/>
-        <v>101812</v>
+        <v>101810</v>
       </c>
       <c r="C143">
         <v>240</v>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="B144">
         <f t="shared" si="4"/>
-        <v>101987</v>
+        <v>101985</v>
       </c>
       <c r="C144">
         <v>175</v>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B145">
         <f t="shared" si="4"/>
-        <v>102080</v>
+        <v>102078</v>
       </c>
       <c r="C145">
         <v>93</v>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="B146">
         <f t="shared" si="4"/>
-        <v>102159</v>
+        <v>102157</v>
       </c>
       <c r="C146">
         <v>79</v>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="B147">
         <f t="shared" si="4"/>
-        <v>102384</v>
+        <v>102382</v>
       </c>
       <c r="C147">
         <v>225</v>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B148">
         <f t="shared" si="4"/>
-        <v>102573</v>
+        <v>102571</v>
       </c>
       <c r="C148">
         <v>189</v>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="B149">
         <f t="shared" si="4"/>
-        <v>102783</v>
+        <v>102781</v>
       </c>
       <c r="C149">
         <v>210</v>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="B150">
         <f t="shared" si="4"/>
-        <v>102989</v>
+        <v>102987</v>
       </c>
       <c r="C150">
         <v>206</v>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="B151">
         <f t="shared" si="4"/>
-        <v>103187</v>
+        <v>103185</v>
       </c>
       <c r="C151">
         <v>198</v>
@@ -3293,7 +3293,7 @@
       </c>
       <c r="B152">
         <f t="shared" si="4"/>
-        <v>103321</v>
+        <v>103319</v>
       </c>
       <c r="C152">
         <v>134</v>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="B153">
         <f t="shared" si="4"/>
-        <v>103392</v>
+        <v>103390</v>
       </c>
       <c r="C153">
         <v>71</v>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="B154">
         <f t="shared" si="4"/>
-        <v>103597</v>
+        <v>103595</v>
       </c>
       <c r="C154">
         <v>205</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B155">
         <f t="shared" si="4"/>
-        <v>103817</v>
+        <v>103815</v>
       </c>
       <c r="C155">
         <v>220</v>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="B156">
         <f t="shared" si="4"/>
-        <v>104033</v>
+        <v>104031</v>
       </c>
       <c r="C156">
         <v>216</v>
@@ -3373,7 +3373,7 @@
       </c>
       <c r="B157">
         <f t="shared" si="4"/>
-        <v>104259</v>
+        <v>104257</v>
       </c>
       <c r="C157">
         <v>226</v>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="B158">
         <f t="shared" si="4"/>
-        <v>104358</v>
+        <v>104356</v>
       </c>
       <c r="C158">
         <v>99</v>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="B159">
         <f t="shared" si="4"/>
-        <v>104418</v>
+        <v>104416</v>
       </c>
       <c r="C159">
         <v>60</v>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B160">
         <f t="shared" si="4"/>
-        <v>104519</v>
+        <v>104517</v>
       </c>
       <c r="C160">
         <v>101</v>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B161">
         <f t="shared" si="4"/>
-        <v>104756</v>
+        <v>104754</v>
       </c>
       <c r="C161">
         <v>237</v>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="B162">
         <f t="shared" si="4"/>
-        <v>104998</v>
+        <v>104996</v>
       </c>
       <c r="C162">
         <v>242</v>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="B163">
         <f t="shared" si="4"/>
-        <v>105214</v>
+        <v>105212</v>
       </c>
       <c r="C163">
         <v>216</v>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="B164">
         <f t="shared" si="4"/>
-        <v>105468</v>
+        <v>105466</v>
       </c>
       <c r="C164">
         <v>254</v>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B165">
         <f t="shared" si="4"/>
-        <v>105696</v>
+        <v>105694</v>
       </c>
       <c r="C165">
         <v>228</v>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="B166">
         <f t="shared" si="4"/>
-        <v>105813</v>
+        <v>105811</v>
       </c>
       <c r="C166">
         <v>117</v>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="B167">
         <f t="shared" si="4"/>
-        <v>105900</v>
+        <v>105898</v>
       </c>
       <c r="C167">
         <v>87</v>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="B168">
         <f t="shared" si="4"/>
-        <v>106166</v>
+        <v>106164</v>
       </c>
       <c r="C168">
         <v>266</v>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="B169">
         <f t="shared" si="4"/>
-        <v>106398</v>
+        <v>106396</v>
       </c>
       <c r="C169">
         <v>232</v>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B170">
         <f t="shared" si="4"/>
-        <v>106696</v>
+        <v>106694</v>
       </c>
       <c r="C170">
         <v>298</v>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B171">
         <f t="shared" si="4"/>
-        <v>106940</v>
+        <v>106938</v>
       </c>
       <c r="C171">
         <v>244</v>
@@ -3613,7 +3613,7 @@
       </c>
       <c r="B172">
         <f t="shared" si="4"/>
-        <v>107167</v>
+        <v>107165</v>
       </c>
       <c r="C172">
         <v>227</v>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="B173">
         <f t="shared" si="4"/>
-        <v>107295</v>
+        <v>107293</v>
       </c>
       <c r="C173">
         <v>128</v>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B174">
         <f t="shared" si="4"/>
-        <v>107369</v>
+        <v>107367</v>
       </c>
       <c r="C174">
         <v>74</v>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="B175">
         <f t="shared" si="4"/>
-        <v>107648</v>
+        <v>107646</v>
       </c>
       <c r="C175">
         <v>279</v>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B176">
         <f t="shared" si="4"/>
-        <v>107903</v>
+        <v>107901</v>
       </c>
       <c r="C176">
         <v>255</v>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="B177">
         <f t="shared" si="4"/>
-        <v>108161</v>
+        <v>108159</v>
       </c>
       <c r="C177">
         <v>258</v>
@@ -3709,7 +3709,7 @@
       </c>
       <c r="B178">
         <f t="shared" si="4"/>
-        <v>108420</v>
+        <v>108418</v>
       </c>
       <c r="C178">
         <v>259</v>
@@ -3725,7 +3725,7 @@
       </c>
       <c r="B179">
         <f t="shared" si="4"/>
-        <v>108678</v>
+        <v>108676</v>
       </c>
       <c r="C179">
         <v>258</v>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B180">
         <f t="shared" si="4"/>
-        <v>108837</v>
+        <v>108835</v>
       </c>
       <c r="C180">
         <v>159</v>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="B181">
         <f t="shared" si="4"/>
-        <v>108938</v>
+        <v>108936</v>
       </c>
       <c r="C181">
         <v>101</v>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B182">
         <f t="shared" si="4"/>
-        <v>109299</v>
+        <v>109297</v>
       </c>
       <c r="C182">
         <v>361</v>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="B183">
         <f t="shared" si="4"/>
-        <v>109619</v>
+        <v>109617</v>
       </c>
       <c r="C183">
         <v>320</v>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="B184">
         <f t="shared" si="4"/>
-        <v>109938</v>
+        <v>109936</v>
       </c>
       <c r="C184">
         <v>319</v>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="B185">
         <f t="shared" si="4"/>
-        <v>110274</v>
+        <v>110272</v>
       </c>
       <c r="C185">
         <v>336</v>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B186">
         <f t="shared" si="4"/>
-        <v>110593</v>
+        <v>110591</v>
       </c>
       <c r="C186">
         <v>319</v>
@@ -3853,7 +3853,7 @@
       </c>
       <c r="B187">
         <f t="shared" si="4"/>
-        <v>110740</v>
+        <v>110738</v>
       </c>
       <c r="C187">
         <v>147</v>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="B188">
         <f t="shared" si="4"/>
-        <v>110849</v>
+        <v>110847</v>
       </c>
       <c r="C188">
         <v>109</v>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B189">
         <f t="shared" si="4"/>
-        <v>111208</v>
+        <v>111206</v>
       </c>
       <c r="C189">
         <v>359</v>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="B190">
         <f t="shared" si="4"/>
-        <v>111516</v>
+        <v>111514</v>
       </c>
       <c r="C190">
         <v>308</v>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="B191">
         <f t="shared" si="4"/>
-        <v>111849</v>
+        <v>111847</v>
       </c>
       <c r="C191">
         <v>333</v>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="B192">
         <f t="shared" si="4"/>
-        <v>112203</v>
+        <v>112201</v>
       </c>
       <c r="C192">
         <v>354</v>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="B193">
         <f t="shared" si="4"/>
-        <v>112502</v>
+        <v>112500</v>
       </c>
       <c r="C193">
         <v>299</v>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="B194">
         <f t="shared" si="4"/>
-        <v>112671</v>
+        <v>112669</v>
       </c>
       <c r="C194">
         <v>169</v>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B195">
         <f t="shared" si="4"/>
-        <v>112756</v>
+        <v>112754</v>
       </c>
       <c r="C195">
         <v>85</v>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="B196">
         <f t="shared" ref="B196:B259" si="6">C196+B195</f>
-        <v>113130</v>
+        <v>113128</v>
       </c>
       <c r="C196">
         <v>374</v>
@@ -4013,14 +4013,14 @@
       </c>
       <c r="B197">
         <f t="shared" si="6"/>
-        <v>113415</v>
+        <v>113412</v>
       </c>
       <c r="C197">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D197">
         <f t="shared" si="5"/>
-        <v>271.28571428571428</v>
+        <v>271.14285714285717</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4029,14 +4029,14 @@
       </c>
       <c r="B198">
         <f t="shared" si="6"/>
-        <v>113719</v>
+        <v>113716</v>
       </c>
       <c r="C198">
         <v>304</v>
       </c>
       <c r="D198">
         <f t="shared" si="5"/>
-        <v>267.14285714285717</v>
+        <v>267</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4045,14 +4045,14 @@
       </c>
       <c r="B199">
         <f t="shared" si="6"/>
-        <v>114068</v>
+        <v>114065</v>
       </c>
       <c r="C199">
         <v>349</v>
       </c>
       <c r="D199">
         <f t="shared" si="5"/>
-        <v>266.42857142857144</v>
+        <v>266.28571428571428</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4061,14 +4061,14 @@
       </c>
       <c r="B200">
         <f t="shared" si="6"/>
-        <v>114410</v>
+        <v>114407</v>
       </c>
       <c r="C200">
         <v>342</v>
       </c>
       <c r="D200">
         <f t="shared" si="5"/>
-        <v>272.57142857142856</v>
+        <v>272.42857142857144</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,14 +4077,14 @@
       </c>
       <c r="B201">
         <f t="shared" si="6"/>
-        <v>114561</v>
+        <v>114558</v>
       </c>
       <c r="C201">
         <v>151</v>
       </c>
       <c r="D201">
         <f t="shared" ref="D201:D264" si="7">AVERAGE(C195:C201)</f>
-        <v>270</v>
+        <v>269.85714285714283</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4093,14 +4093,14 @@
       </c>
       <c r="B202">
         <f t="shared" si="6"/>
-        <v>114681</v>
+        <v>114678</v>
       </c>
       <c r="C202">
         <v>120</v>
       </c>
       <c r="D202">
         <f t="shared" si="7"/>
-        <v>275</v>
+        <v>274.85714285714283</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4109,14 +4109,14 @@
       </c>
       <c r="B203">
         <f t="shared" si="6"/>
-        <v>115050</v>
+        <v>115047</v>
       </c>
       <c r="C203">
         <v>369</v>
       </c>
       <c r="D203">
         <f t="shared" si="7"/>
-        <v>274.28571428571428</v>
+        <v>274.14285714285717</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B204">
         <f t="shared" si="6"/>
-        <v>115431</v>
+        <v>115428</v>
       </c>
       <c r="C204">
         <v>381</v>
@@ -4141,7 +4141,7 @@
       </c>
       <c r="B205">
         <f t="shared" si="6"/>
-        <v>115769</v>
+        <v>115766</v>
       </c>
       <c r="C205">
         <v>338</v>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="B206">
         <f t="shared" si="6"/>
-        <v>116125</v>
+        <v>116122</v>
       </c>
       <c r="C206">
         <v>356</v>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="B207">
         <f t="shared" si="6"/>
-        <v>116408</v>
+        <v>116405</v>
       </c>
       <c r="C207">
         <v>283</v>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="B208">
         <f t="shared" si="6"/>
-        <v>116557</v>
+        <v>116554</v>
       </c>
       <c r="C208">
         <v>149</v>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="B209">
         <f t="shared" si="6"/>
-        <v>116649</v>
+        <v>116646</v>
       </c>
       <c r="C209">
         <v>92</v>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B210">
         <f t="shared" si="6"/>
-        <v>117045</v>
+        <v>117042</v>
       </c>
       <c r="C210">
         <v>396</v>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="B211">
         <f t="shared" si="6"/>
-        <v>117425</v>
+        <v>117422</v>
       </c>
       <c r="C211">
         <v>380</v>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="B212">
         <f t="shared" si="6"/>
-        <v>117804</v>
+        <v>117801</v>
       </c>
       <c r="C212">
         <v>379</v>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="B213">
         <f t="shared" si="6"/>
-        <v>118149</v>
+        <v>118146</v>
       </c>
       <c r="C213">
         <v>345</v>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="B214">
         <f t="shared" si="6"/>
-        <v>118513</v>
+        <v>118510</v>
       </c>
       <c r="C214">
         <v>364</v>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="B215">
         <f t="shared" si="6"/>
-        <v>118685</v>
+        <v>118682</v>
       </c>
       <c r="C215">
         <v>172</v>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="B216">
         <f t="shared" si="6"/>
-        <v>118824</v>
+        <v>118821</v>
       </c>
       <c r="C216">
         <v>139</v>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="B217">
         <f t="shared" si="6"/>
-        <v>119262</v>
+        <v>119259</v>
       </c>
       <c r="C217">
         <v>438</v>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="B218">
         <f t="shared" si="6"/>
-        <v>119657</v>
+        <v>119654</v>
       </c>
       <c r="C218">
         <v>395</v>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="B219">
         <f t="shared" si="6"/>
-        <v>120041</v>
+        <v>120038</v>
       </c>
       <c r="C219">
         <v>384</v>
@@ -4381,7 +4381,7 @@
       </c>
       <c r="B220">
         <f t="shared" si="6"/>
-        <v>120505</v>
+        <v>120502</v>
       </c>
       <c r="C220">
         <v>464</v>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="B221">
         <f t="shared" si="6"/>
-        <v>120853</v>
+        <v>120850</v>
       </c>
       <c r="C221">
         <v>348</v>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="B222">
         <f t="shared" si="6"/>
-        <v>121051</v>
+        <v>121048</v>
       </c>
       <c r="C222">
         <v>198</v>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="B223">
         <f t="shared" si="6"/>
-        <v>121163</v>
+        <v>121160</v>
       </c>
       <c r="C223">
         <v>112</v>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="B224">
         <f t="shared" si="6"/>
-        <v>121324</v>
+        <v>121321</v>
       </c>
       <c r="C224">
         <v>161</v>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="B225">
         <f t="shared" si="6"/>
-        <v>121871</v>
+        <v>121868</v>
       </c>
       <c r="C225">
         <v>547</v>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="B226">
         <f t="shared" si="6"/>
-        <v>122345</v>
+        <v>122342</v>
       </c>
       <c r="C226">
         <v>474</v>
@@ -4493,7 +4493,7 @@
       </c>
       <c r="B227">
         <f t="shared" si="6"/>
-        <v>122755</v>
+        <v>122752</v>
       </c>
       <c r="C227">
         <v>410</v>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B228">
         <f t="shared" si="6"/>
-        <v>123164</v>
+        <v>123161</v>
       </c>
       <c r="C228">
         <v>409</v>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="B229">
         <f t="shared" si="6"/>
-        <v>123353</v>
+        <v>123350</v>
       </c>
       <c r="C229">
         <v>189</v>
@@ -4541,7 +4541,7 @@
       </c>
       <c r="B230">
         <f t="shared" si="6"/>
-        <v>123514</v>
+        <v>123511</v>
       </c>
       <c r="C230">
         <v>161</v>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="B231">
         <f t="shared" si="6"/>
-        <v>124018</v>
+        <v>124015</v>
       </c>
       <c r="C231">
         <v>504</v>
@@ -4573,14 +4573,14 @@
       </c>
       <c r="B232">
         <f t="shared" si="6"/>
-        <v>124439</v>
+        <v>124438</v>
       </c>
       <c r="C232">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D232">
         <f t="shared" si="7"/>
-        <v>366.85714285714283</v>
+        <v>367.14285714285717</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -4589,14 +4589,14 @@
       </c>
       <c r="B233">
         <f t="shared" si="6"/>
-        <v>124853</v>
+        <v>124852</v>
       </c>
       <c r="C233">
         <v>414</v>
       </c>
       <c r="D233">
         <f t="shared" si="7"/>
-        <v>358.28571428571428</v>
+        <v>358.57142857142856</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -4605,14 +4605,14 @@
       </c>
       <c r="B234">
         <f t="shared" si="6"/>
-        <v>125208</v>
+        <v>125207</v>
       </c>
       <c r="C234">
         <v>355</v>
       </c>
       <c r="D234">
         <f t="shared" si="7"/>
-        <v>350.42857142857144</v>
+        <v>350.71428571428572</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -4621,14 +4621,14 @@
       </c>
       <c r="B235">
         <f t="shared" si="6"/>
-        <v>125643</v>
+        <v>125642</v>
       </c>
       <c r="C235">
         <v>435</v>
       </c>
       <c r="D235">
         <f t="shared" si="7"/>
-        <v>354.14285714285717</v>
+        <v>354.42857142857144</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -4637,14 +4637,14 @@
       </c>
       <c r="B236">
         <f t="shared" si="6"/>
-        <v>125845</v>
+        <v>125844</v>
       </c>
       <c r="C236">
         <v>202</v>
       </c>
       <c r="D236">
         <f t="shared" si="7"/>
-        <v>356</v>
+        <v>356.28571428571428</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -4653,14 +4653,14 @@
       </c>
       <c r="B237">
         <f t="shared" si="6"/>
-        <v>125987</v>
+        <v>125986</v>
       </c>
       <c r="C237">
         <v>142</v>
       </c>
       <c r="D237">
         <f t="shared" si="7"/>
-        <v>353.28571428571428</v>
+        <v>353.57142857142856</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -4669,14 +4669,14 @@
       </c>
       <c r="B238">
         <f t="shared" si="6"/>
-        <v>126414</v>
+        <v>126413</v>
       </c>
       <c r="C238">
         <v>427</v>
       </c>
       <c r="D238">
         <f t="shared" si="7"/>
-        <v>342.28571428571428</v>
+        <v>342.57142857142856</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -4685,7 +4685,7 @@
       </c>
       <c r="B239">
         <f t="shared" si="6"/>
-        <v>126923</v>
+        <v>126922</v>
       </c>
       <c r="C239">
         <v>509</v>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B240">
         <f t="shared" si="6"/>
-        <v>127483</v>
+        <v>127482</v>
       </c>
       <c r="C240">
         <v>560</v>
@@ -4717,7 +4717,7 @@
       </c>
       <c r="B241">
         <f t="shared" si="6"/>
-        <v>128081</v>
+        <v>128080</v>
       </c>
       <c r="C241">
         <v>598</v>
@@ -4733,7 +4733,7 @@
       </c>
       <c r="B242">
         <f t="shared" si="6"/>
-        <v>128634</v>
+        <v>128633</v>
       </c>
       <c r="C242">
         <v>553</v>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="B243">
         <f t="shared" si="6"/>
-        <v>128998</v>
+        <v>128997</v>
       </c>
       <c r="C243">
         <v>364</v>
@@ -4765,7 +4765,7 @@
       </c>
       <c r="B244">
         <f t="shared" si="6"/>
-        <v>129222</v>
+        <v>129221</v>
       </c>
       <c r="C244">
         <v>224</v>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="B245">
         <f t="shared" si="6"/>
-        <v>130089</v>
+        <v>130088</v>
       </c>
       <c r="C245">
         <v>867</v>
@@ -4800,11 +4800,11 @@
         <v>130807</v>
       </c>
       <c r="C246">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D246">
         <f t="shared" si="7"/>
-        <v>554.85714285714289</v>
+        <v>555</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -4820,7 +4820,7 @@
       </c>
       <c r="D247">
         <f t="shared" si="7"/>
-        <v>562.42857142857144</v>
+        <v>562.57142857142856</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="D248">
         <f t="shared" si="7"/>
-        <v>574.57142857142856</v>
+        <v>574.71428571428567</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
       </c>
       <c r="D249">
         <f t="shared" si="7"/>
-        <v>576.42857142857144</v>
+        <v>576.57142857142856</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -4868,7 +4868,7 @@
       </c>
       <c r="D250">
         <f t="shared" si="7"/>
-        <v>582.71428571428567</v>
+        <v>582.85714285714289</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -4884,7 +4884,7 @@
       </c>
       <c r="D251">
         <f t="shared" si="7"/>
-        <v>592.42857142857144</v>
+        <v>592.57142857142856</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -4900,7 +4900,7 @@
       </c>
       <c r="D252">
         <f t="shared" si="7"/>
-        <v>575.85714285714289</v>
+        <v>576</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -5341,14 +5341,14 @@
       </c>
       <c r="B280">
         <f t="shared" si="8"/>
-        <v>160084</v>
+        <v>160085</v>
       </c>
       <c r="C280">
-        <v>1839</v>
+        <v>1840</v>
       </c>
       <c r="D280">
-        <f t="shared" ref="D280:D312" si="10">AVERAGE(C274:C280)</f>
-        <v>1219</v>
+        <f t="shared" ref="D280:D313" si="10">AVERAGE(C274:C280)</f>
+        <v>1219.1428571428571</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -5357,14 +5357,14 @@
       </c>
       <c r="B281">
         <f t="shared" si="8"/>
-        <v>161995</v>
+        <v>161996</v>
       </c>
       <c r="C281">
         <v>1911</v>
       </c>
       <c r="D281">
         <f t="shared" si="10"/>
-        <v>1299.7142857142858</v>
+        <v>1299.8571428571429</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -5373,14 +5373,14 @@
       </c>
       <c r="B282">
         <f t="shared" si="8"/>
-        <v>164174</v>
+        <v>164175</v>
       </c>
       <c r="C282">
         <v>2179</v>
       </c>
       <c r="D282">
         <f t="shared" si="10"/>
-        <v>1404.8571428571429</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -5389,14 +5389,14 @@
       </c>
       <c r="B283">
         <f t="shared" si="8"/>
-        <v>166590</v>
+        <v>166595</v>
       </c>
       <c r="C283">
-        <v>2416</v>
+        <v>2420</v>
       </c>
       <c r="D283">
         <f t="shared" si="10"/>
-        <v>1552</v>
+        <v>1552.7142857142858</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -5405,14 +5405,14 @@
       </c>
       <c r="B284">
         <f t="shared" si="8"/>
-        <v>168828</v>
+        <v>168834</v>
       </c>
       <c r="C284">
-        <v>2238</v>
+        <v>2239</v>
       </c>
       <c r="D284">
         <f t="shared" si="10"/>
-        <v>1711</v>
+        <v>1711.8571428571429</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
@@ -5421,14 +5421,14 @@
       </c>
       <c r="B285">
         <f t="shared" si="8"/>
-        <v>170155</v>
+        <v>170161</v>
       </c>
       <c r="C285">
         <v>1327</v>
       </c>
       <c r="D285">
         <f t="shared" si="10"/>
-        <v>1776</v>
+        <v>1776.8571428571429</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -5437,14 +5437,14 @@
       </c>
       <c r="B286">
         <f t="shared" si="8"/>
-        <v>171098</v>
+        <v>171103</v>
       </c>
       <c r="C286">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D286">
         <f t="shared" si="10"/>
-        <v>1836.1428571428571</v>
+        <v>1836.8571428571429</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
@@ -5452,15 +5452,15 @@
         <v>44144</v>
       </c>
       <c r="B287">
-        <f t="shared" ref="B287:B312" si="11">C287+B286</f>
-        <v>174278</v>
+        <f t="shared" ref="B287:B313" si="11">C287+B286</f>
+        <v>174282</v>
       </c>
       <c r="C287">
-        <v>3180</v>
+        <v>3179</v>
       </c>
       <c r="D287">
         <f t="shared" si="10"/>
-        <v>2027.7142857142858</v>
+        <v>2028.1428571428571</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
@@ -5469,14 +5469,14 @@
       </c>
       <c r="B288">
         <f t="shared" si="11"/>
-        <v>177102</v>
+        <v>177106</v>
       </c>
       <c r="C288">
         <v>2824</v>
       </c>
       <c r="D288">
         <f t="shared" si="10"/>
-        <v>2158.1428571428573</v>
+        <v>2158.5714285714284</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -5485,14 +5485,14 @@
       </c>
       <c r="B289">
         <f t="shared" si="11"/>
-        <v>179767</v>
+        <v>179771</v>
       </c>
       <c r="C289">
         <v>2665</v>
       </c>
       <c r="D289">
         <f t="shared" si="10"/>
-        <v>2227.5714285714284</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -5501,14 +5501,14 @@
       </c>
       <c r="B290">
         <f t="shared" si="11"/>
-        <v>182760</v>
+        <v>182764</v>
       </c>
       <c r="C290">
         <v>2993</v>
       </c>
       <c r="D290">
         <f t="shared" si="10"/>
-        <v>2310</v>
+        <v>2309.8571428571427</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -5517,14 +5517,14 @@
       </c>
       <c r="B291">
         <f t="shared" si="11"/>
-        <v>185369</v>
+        <v>185373</v>
       </c>
       <c r="C291">
         <v>2609</v>
       </c>
       <c r="D291">
         <f t="shared" si="10"/>
-        <v>2363</v>
+        <v>2362.7142857142858</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -5533,14 +5533,14 @@
       </c>
       <c r="B292">
         <f t="shared" si="11"/>
-        <v>187084</v>
+        <v>187087</v>
       </c>
       <c r="C292">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D292">
         <f t="shared" si="10"/>
-        <v>2418.4285714285716</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -5549,14 +5549,14 @@
       </c>
       <c r="B293">
         <f t="shared" si="11"/>
-        <v>188279</v>
+        <v>188282</v>
       </c>
       <c r="C293">
         <v>1195</v>
       </c>
       <c r="D293">
         <f t="shared" si="10"/>
-        <v>2454.4285714285716</v>
+        <v>2454.1428571428573</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
@@ -5565,14 +5565,14 @@
       </c>
       <c r="B294">
         <f t="shared" si="11"/>
-        <v>191801</v>
+        <v>191804</v>
       </c>
       <c r="C294">
         <v>3522</v>
       </c>
       <c r="D294">
         <f>AVERAGE(C288:C294)</f>
-        <v>2503.2857142857142</v>
+        <v>2503.1428571428573</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -5581,14 +5581,14 @@
       </c>
       <c r="B295">
         <f t="shared" si="11"/>
-        <v>194937</v>
+        <v>194939</v>
       </c>
       <c r="C295">
-        <v>3136</v>
+        <v>3135</v>
       </c>
       <c r="D295">
         <f t="shared" si="10"/>
-        <v>2547.8571428571427</v>
+        <v>2547.5714285714284</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
@@ -5600,11 +5600,11 @@
         <v>197858</v>
       </c>
       <c r="C296">
-        <v>2921</v>
+        <v>2919</v>
       </c>
       <c r="D296">
         <f t="shared" si="10"/>
-        <v>2584.4285714285716</v>
+        <v>2583.8571428571427</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
@@ -5613,14 +5613,14 @@
       </c>
       <c r="B297">
         <f t="shared" si="11"/>
-        <v>200860</v>
+        <v>200858</v>
       </c>
       <c r="C297">
-        <v>3002</v>
+        <v>3000</v>
       </c>
       <c r="D297">
         <f t="shared" si="10"/>
-        <v>2585.7142857142858</v>
+        <v>2584.8571428571427</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -5629,14 +5629,14 @@
       </c>
       <c r="B298">
         <f t="shared" si="11"/>
-        <v>203721</v>
+        <v>203717</v>
       </c>
       <c r="C298">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="D298">
         <f t="shared" si="10"/>
-        <v>2621.7142857142858</v>
+        <v>2620.5714285714284</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -5645,14 +5645,14 @@
       </c>
       <c r="B299">
         <f t="shared" si="11"/>
-        <v>205493</v>
+        <v>205489</v>
       </c>
       <c r="C299">
         <v>1772</v>
       </c>
       <c r="D299">
         <f t="shared" si="10"/>
-        <v>2629.8571428571427</v>
+        <v>2628.8571428571427</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -5661,14 +5661,14 @@
       </c>
       <c r="B300">
         <f t="shared" si="11"/>
-        <v>206681</v>
+        <v>206676</v>
       </c>
       <c r="C300">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="D300">
         <f t="shared" si="10"/>
-        <v>2628.8571428571427</v>
+        <v>2627.7142857142858</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -5677,14 +5677,14 @@
       </c>
       <c r="B301">
         <f t="shared" si="11"/>
-        <v>210279</v>
+        <v>210272</v>
       </c>
       <c r="C301">
-        <v>3598</v>
+        <v>3596</v>
       </c>
       <c r="D301">
         <f t="shared" si="10"/>
-        <v>2639.7142857142858</v>
+        <v>2638.2857142857142</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
@@ -5693,14 +5693,14 @@
       </c>
       <c r="B302">
         <f t="shared" si="11"/>
-        <v>214069</v>
+        <v>214062</v>
       </c>
       <c r="C302">
         <v>3790</v>
       </c>
       <c r="D302">
         <f t="shared" si="10"/>
-        <v>2733.1428571428573</v>
+        <v>2731.8571428571427</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
@@ -5709,14 +5709,14 @@
       </c>
       <c r="B303">
         <f t="shared" si="11"/>
-        <v>217013</v>
+        <v>217008</v>
       </c>
       <c r="C303">
-        <v>2944</v>
+        <v>2946</v>
       </c>
       <c r="D303">
         <f t="shared" si="10"/>
-        <v>2736.4285714285716</v>
+        <v>2735.7142857142858</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
@@ -5725,14 +5725,14 @@
       </c>
       <c r="B304">
         <f t="shared" si="11"/>
-        <v>217458</v>
+        <v>217453</v>
       </c>
       <c r="C304">
         <v>445</v>
       </c>
       <c r="D304">
         <f t="shared" si="10"/>
-        <v>2371.1428571428573</v>
+        <v>2370.7142857142858</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
@@ -5744,11 +5744,11 @@
         <v>220816</v>
       </c>
       <c r="C305">
-        <v>3358</v>
+        <v>3363</v>
       </c>
       <c r="D305">
         <f t="shared" si="10"/>
-        <v>2442.1428571428573</v>
+        <v>2442.7142857142858</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -5757,14 +5757,14 @@
       </c>
       <c r="B306">
         <f t="shared" si="11"/>
-        <v>223715</v>
+        <v>223718</v>
       </c>
       <c r="C306">
-        <v>2899</v>
+        <v>2902</v>
       </c>
       <c r="D306">
         <f t="shared" si="10"/>
-        <v>2603.1428571428573</v>
+        <v>2604.1428571428573</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -5773,14 +5773,14 @@
       </c>
       <c r="B307">
         <f t="shared" si="11"/>
-        <v>225403</v>
+        <v>225445</v>
       </c>
       <c r="C307">
-        <v>1688</v>
+        <v>1727</v>
       </c>
       <c r="D307">
         <f t="shared" si="10"/>
-        <v>2674.5714285714284</v>
+        <v>2681.2857142857142</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -5789,14 +5789,14 @@
       </c>
       <c r="B308">
         <f t="shared" si="11"/>
-        <v>230444</v>
+        <v>230739</v>
       </c>
       <c r="C308">
-        <v>5041</v>
+        <v>5294</v>
       </c>
       <c r="D308">
         <f t="shared" si="10"/>
-        <v>2880.7142857142858</v>
+        <v>2923.8571428571427</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -5805,14 +5805,14 @@
       </c>
       <c r="B309">
         <f t="shared" si="11"/>
-        <v>235464</v>
+        <v>236187</v>
       </c>
       <c r="C309">
-        <v>5020</v>
+        <v>5448</v>
       </c>
       <c r="D309">
         <f t="shared" si="10"/>
-        <v>3056.4285714285716</v>
+        <v>3160.7142857142858</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -5821,14 +5821,14 @@
       </c>
       <c r="B310">
         <f t="shared" si="11"/>
-        <v>239583</v>
+        <v>240949</v>
       </c>
       <c r="C310">
-        <v>4119</v>
+        <v>4762</v>
       </c>
       <c r="D310">
         <f t="shared" si="10"/>
-        <v>3224.2857142857142</v>
+        <v>3420.1428571428573</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -5837,14 +5837,14 @@
       </c>
       <c r="B311">
         <f t="shared" si="11"/>
-        <v>242680</v>
+        <v>244877</v>
       </c>
       <c r="C311">
-        <v>3097</v>
+        <v>3928</v>
       </c>
       <c r="D311">
         <f t="shared" si="10"/>
-        <v>3603.1428571428573</v>
+        <v>3917.7142857142858</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -5853,14 +5853,30 @@
       </c>
       <c r="B312">
         <f t="shared" si="11"/>
-        <v>242812</v>
+        <v>247474</v>
       </c>
       <c r="C312">
-        <v>132</v>
+        <v>2597</v>
       </c>
       <c r="D312">
         <f t="shared" si="10"/>
-        <v>3142.2857142857142</v>
+        <v>3808.2857142857142</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" s="1">
+        <v>44170</v>
+      </c>
+      <c r="B313">
+        <f t="shared" si="11"/>
+        <v>247559</v>
+      </c>
+      <c r="C313">
+        <v>85</v>
+      </c>
+      <c r="D313">
+        <f t="shared" si="10"/>
+        <v>3405.8571428571427</v>
       </c>
     </row>
   </sheetData>
@@ -5878,12 +5894,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008004546134034441816F24C41F65E929" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c3392cbe151f976ef883c2eee1f53348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0967b7be50301903c78f9c39c6fd9af8">
     <xsd:element name="properties">
@@ -5997,6 +6007,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C76A581D-70D9-4324-B3C2-C549CBC3A500}">
   <ds:schemaRefs>
@@ -6006,15 +6022,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E2A907-BC75-4262-BBD0-4F1B2976CD82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A7812BB-980B-4585-92C6-973734300155}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6028,4 +6035,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E2A907-BC75-4262-BBD0-4F1B2976CD82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update of daily and weekly charts
</commit_message>
<xml_diff>
--- a/data/CasesByDate.xlsx
+++ b/data/CasesByDate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\COVID-19 Data Visualization\COVID19 - Files\Power BI resources\CSV filesPROB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAF4470-FF08-4953-98B2-F059FB7BD44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD2D6C2-2960-4061-A5DC-496A04F125CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29280" yWindow="480" windowWidth="21600" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CasesByDate" sheetId="1" r:id="rId1"/>
@@ -884,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D316"/>
+  <dimension ref="A1:D317"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B302" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B311" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B324" sqref="B324"/>
@@ -2240,14 +2240,14 @@
       </c>
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>51241</v>
+        <v>51242</v>
       </c>
       <c r="C86">
-        <v>2703</v>
+        <v>2704</v>
       </c>
       <c r="D86">
         <f t="shared" si="3"/>
-        <v>2217</v>
+        <v>2217.1428571428573</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2256,14 +2256,14 @@
       </c>
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>53646</v>
+        <v>53647</v>
       </c>
       <c r="C87">
         <v>2405</v>
       </c>
       <c r="D87">
         <f t="shared" si="3"/>
-        <v>2219.7142857142858</v>
+        <v>2219.8571428571427</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2272,14 +2272,14 @@
       </c>
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>55920</v>
+        <v>55921</v>
       </c>
       <c r="C88">
         <v>2274</v>
       </c>
       <c r="D88">
         <f t="shared" si="3"/>
-        <v>2117.5714285714284</v>
+        <v>2117.7142857142858</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2288,14 +2288,14 @@
       </c>
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>57412</v>
+        <v>57413</v>
       </c>
       <c r="C89">
         <v>1492</v>
       </c>
       <c r="D89">
         <f t="shared" si="3"/>
-        <v>2119.2857142857142</v>
+        <v>2119.4285714285716</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2304,14 +2304,14 @@
       </c>
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>58256</v>
+        <v>58257</v>
       </c>
       <c r="C90">
         <v>844</v>
       </c>
       <c r="D90">
         <f t="shared" si="3"/>
-        <v>2084.2857142857142</v>
+        <v>2084.4285714285716</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2320,14 +2320,14 @@
       </c>
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>60384</v>
+        <v>60385</v>
       </c>
       <c r="C91">
         <v>2128</v>
       </c>
       <c r="D91">
         <f t="shared" si="3"/>
-        <v>2004.5714285714287</v>
+        <v>2004.7142857142858</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2336,14 +2336,14 @@
       </c>
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>62487</v>
+        <v>62488</v>
       </c>
       <c r="C92">
         <v>2103</v>
       </c>
       <c r="D92">
         <f t="shared" si="3"/>
-        <v>1992.7142857142858</v>
+        <v>1992.8571428571429</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>64673</v>
+        <v>64674</v>
       </c>
       <c r="C93">
         <v>2186</v>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>66720</v>
+        <v>66721</v>
       </c>
       <c r="C94">
         <v>2047</v>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>68801</v>
+        <v>68802</v>
       </c>
       <c r="C95">
         <v>2081</v>
@@ -2400,7 +2400,7 @@
       </c>
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>69830</v>
+        <v>69831</v>
       </c>
       <c r="C96">
         <v>1029</v>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>70563</v>
+        <v>70564</v>
       </c>
       <c r="C97">
         <v>733</v>
@@ -2432,7 +2432,7 @@
       </c>
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>72441</v>
+        <v>72442</v>
       </c>
       <c r="C98">
         <v>1878</v>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>74175</v>
+        <v>74176</v>
       </c>
       <c r="C99">
         <v>1734</v>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>75873</v>
+        <v>75874</v>
       </c>
       <c r="C100">
         <v>1698</v>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>77550</v>
+        <v>77551</v>
       </c>
       <c r="C101">
         <v>1677</v>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>79004</v>
+        <v>79005</v>
       </c>
       <c r="C102">
         <v>1454</v>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>79686</v>
+        <v>79687</v>
       </c>
       <c r="C103">
         <v>682</v>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>80071</v>
+        <v>80072</v>
       </c>
       <c r="C104">
         <v>385</v>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>81377</v>
+        <v>81378</v>
       </c>
       <c r="C105">
         <v>1306</v>
@@ -2560,7 +2560,7 @@
       </c>
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>82827</v>
+        <v>82828</v>
       </c>
       <c r="C106">
         <v>1450</v>
@@ -2576,7 +2576,7 @@
       </c>
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>84138</v>
+        <v>84139</v>
       </c>
       <c r="C107">
         <v>1311</v>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>85453</v>
+        <v>85454</v>
       </c>
       <c r="C108">
         <v>1315</v>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>86558</v>
+        <v>86559</v>
       </c>
       <c r="C109">
         <v>1105</v>
@@ -2624,7 +2624,7 @@
       </c>
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>87203</v>
+        <v>87204</v>
       </c>
       <c r="C110">
         <v>645</v>
@@ -2640,7 +2640,7 @@
       </c>
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>87566</v>
+        <v>87567</v>
       </c>
       <c r="C111">
         <v>363</v>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>88879</v>
+        <v>88880</v>
       </c>
       <c r="C112">
         <v>1313</v>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>89952</v>
+        <v>89953</v>
       </c>
       <c r="C113">
         <v>1073</v>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>90963</v>
+        <v>90964</v>
       </c>
       <c r="C114">
         <v>1011</v>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>91927</v>
+        <v>91928</v>
       </c>
       <c r="C115">
         <v>964</v>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>92789</v>
+        <v>92790</v>
       </c>
       <c r="C116">
         <v>862</v>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>93176</v>
+        <v>93177</v>
       </c>
       <c r="C117">
         <v>387</v>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>93477</v>
+        <v>93478</v>
       </c>
       <c r="C118">
         <v>301</v>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>93675</v>
+        <v>93676</v>
       </c>
       <c r="C119">
         <v>198</v>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>94539</v>
+        <v>94540</v>
       </c>
       <c r="C120">
         <v>864</v>
@@ -2800,7 +2800,7 @@
       </c>
       <c r="B121">
         <f t="shared" si="2"/>
-        <v>95226</v>
+        <v>95227</v>
       </c>
       <c r="C121">
         <v>687</v>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="B122">
         <f t="shared" si="2"/>
-        <v>95865</v>
+        <v>95866</v>
       </c>
       <c r="C122">
         <v>639</v>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="B123">
         <f t="shared" si="2"/>
-        <v>96395</v>
+        <v>96396</v>
       </c>
       <c r="C123">
         <v>530</v>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B124">
         <f t="shared" si="2"/>
-        <v>96666</v>
+        <v>96667</v>
       </c>
       <c r="C124">
         <v>271</v>
@@ -2864,7 +2864,7 @@
       </c>
       <c r="B125">
         <f t="shared" si="2"/>
-        <v>96827</v>
+        <v>96828</v>
       </c>
       <c r="C125">
         <v>161</v>
@@ -2880,7 +2880,7 @@
       </c>
       <c r="B126">
         <f t="shared" si="2"/>
-        <v>97335</v>
+        <v>97336</v>
       </c>
       <c r="C126">
         <v>508</v>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="B127">
         <f t="shared" si="2"/>
-        <v>97782</v>
+        <v>97783</v>
       </c>
       <c r="C127">
         <v>447</v>
@@ -2912,7 +2912,7 @@
       </c>
       <c r="B128">
         <f t="shared" si="2"/>
-        <v>98241</v>
+        <v>98242</v>
       </c>
       <c r="C128">
         <v>459</v>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="B129">
         <f t="shared" si="2"/>
-        <v>98620</v>
+        <v>98621</v>
       </c>
       <c r="C129">
         <v>379</v>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="B130">
         <f t="shared" si="2"/>
-        <v>98957</v>
+        <v>98958</v>
       </c>
       <c r="C130">
         <v>337</v>
@@ -2960,7 +2960,7 @@
       </c>
       <c r="B131">
         <f t="shared" si="2"/>
-        <v>99105</v>
+        <v>99106</v>
       </c>
       <c r="C131">
         <v>148</v>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="B132">
         <f t="shared" ref="B132:B195" si="4">C132+B131</f>
-        <v>99256</v>
+        <v>99257</v>
       </c>
       <c r="C132">
         <v>151</v>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="B133">
         <f t="shared" si="4"/>
-        <v>99609</v>
+        <v>99610</v>
       </c>
       <c r="C133">
         <v>353</v>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="B134">
         <f t="shared" si="4"/>
-        <v>99952</v>
+        <v>99953</v>
       </c>
       <c r="C134">
         <v>343</v>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="B135">
         <f t="shared" si="4"/>
-        <v>100211</v>
+        <v>100212</v>
       </c>
       <c r="C135">
         <v>259</v>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="B136">
         <f t="shared" si="4"/>
-        <v>100437</v>
+        <v>100438</v>
       </c>
       <c r="C136">
         <v>226</v>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="B137">
         <f t="shared" si="4"/>
-        <v>100691</v>
+        <v>100692</v>
       </c>
       <c r="C137">
         <v>254</v>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="B138">
         <f t="shared" si="4"/>
-        <v>100788</v>
+        <v>100789</v>
       </c>
       <c r="C138">
         <v>97</v>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="B139">
         <f t="shared" si="4"/>
-        <v>100864</v>
+        <v>100865</v>
       </c>
       <c r="C139">
         <v>76</v>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="B140">
         <f t="shared" si="4"/>
-        <v>101099</v>
+        <v>101100</v>
       </c>
       <c r="C140">
         <v>235</v>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="B141">
         <f t="shared" si="4"/>
-        <v>101297</v>
+        <v>101298</v>
       </c>
       <c r="C141">
         <v>198</v>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="B142">
         <f t="shared" si="4"/>
-        <v>101546</v>
+        <v>101547</v>
       </c>
       <c r="C142">
         <v>249</v>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="B143">
         <f t="shared" si="4"/>
-        <v>101786</v>
+        <v>101787</v>
       </c>
       <c r="C143">
         <v>240</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="B144">
         <f t="shared" si="4"/>
-        <v>101961</v>
+        <v>101962</v>
       </c>
       <c r="C144">
         <v>175</v>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="B145">
         <f t="shared" si="4"/>
-        <v>102054</v>
+        <v>102055</v>
       </c>
       <c r="C145">
         <v>93</v>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="B146">
         <f t="shared" si="4"/>
-        <v>102133</v>
+        <v>102134</v>
       </c>
       <c r="C146">
         <v>79</v>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="B147">
         <f t="shared" si="4"/>
-        <v>102358</v>
+        <v>102359</v>
       </c>
       <c r="C147">
         <v>225</v>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="B148">
         <f t="shared" si="4"/>
-        <v>102547</v>
+        <v>102548</v>
       </c>
       <c r="C148">
         <v>189</v>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="B149">
         <f t="shared" si="4"/>
-        <v>102757</v>
+        <v>102758</v>
       </c>
       <c r="C149">
         <v>210</v>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="B150">
         <f t="shared" si="4"/>
-        <v>102963</v>
+        <v>102964</v>
       </c>
       <c r="C150">
         <v>206</v>
@@ -3280,7 +3280,7 @@
       </c>
       <c r="B151">
         <f t="shared" si="4"/>
-        <v>103161</v>
+        <v>103162</v>
       </c>
       <c r="C151">
         <v>198</v>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="B152">
         <f t="shared" si="4"/>
-        <v>103295</v>
+        <v>103296</v>
       </c>
       <c r="C152">
         <v>134</v>
@@ -3312,7 +3312,7 @@
       </c>
       <c r="B153">
         <f t="shared" si="4"/>
-        <v>103366</v>
+        <v>103367</v>
       </c>
       <c r="C153">
         <v>71</v>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="B154">
         <f t="shared" si="4"/>
-        <v>103571</v>
+        <v>103572</v>
       </c>
       <c r="C154">
         <v>205</v>
@@ -3344,7 +3344,7 @@
       </c>
       <c r="B155">
         <f t="shared" si="4"/>
-        <v>103791</v>
+        <v>103792</v>
       </c>
       <c r="C155">
         <v>220</v>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="B156">
         <f t="shared" si="4"/>
-        <v>104007</v>
+        <v>104008</v>
       </c>
       <c r="C156">
         <v>216</v>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="B157">
         <f t="shared" si="4"/>
-        <v>104233</v>
+        <v>104234</v>
       </c>
       <c r="C157">
         <v>226</v>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="B158">
         <f t="shared" si="4"/>
-        <v>104332</v>
+        <v>104333</v>
       </c>
       <c r="C158">
         <v>99</v>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="B159">
         <f t="shared" si="4"/>
-        <v>104392</v>
+        <v>104393</v>
       </c>
       <c r="C159">
         <v>60</v>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="B160">
         <f t="shared" si="4"/>
-        <v>104493</v>
+        <v>104494</v>
       </c>
       <c r="C160">
         <v>101</v>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="B161">
         <f t="shared" si="4"/>
-        <v>104730</v>
+        <v>104731</v>
       </c>
       <c r="C161">
         <v>237</v>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="B162">
         <f t="shared" si="4"/>
-        <v>104972</v>
+        <v>104973</v>
       </c>
       <c r="C162">
         <v>242</v>
@@ -3472,7 +3472,7 @@
       </c>
       <c r="B163">
         <f t="shared" si="4"/>
-        <v>105188</v>
+        <v>105189</v>
       </c>
       <c r="C163">
         <v>216</v>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="B164">
         <f t="shared" si="4"/>
-        <v>105442</v>
+        <v>105443</v>
       </c>
       <c r="C164">
         <v>254</v>
@@ -3504,7 +3504,7 @@
       </c>
       <c r="B165">
         <f t="shared" si="4"/>
-        <v>105670</v>
+        <v>105671</v>
       </c>
       <c r="C165">
         <v>228</v>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="B166">
         <f t="shared" si="4"/>
-        <v>105787</v>
+        <v>105788</v>
       </c>
       <c r="C166">
         <v>117</v>
@@ -3536,7 +3536,7 @@
       </c>
       <c r="B167">
         <f t="shared" si="4"/>
-        <v>105874</v>
+        <v>105875</v>
       </c>
       <c r="C167">
         <v>87</v>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="B168">
         <f t="shared" si="4"/>
-        <v>106140</v>
+        <v>106141</v>
       </c>
       <c r="C168">
         <v>266</v>
@@ -3568,7 +3568,7 @@
       </c>
       <c r="B169">
         <f t="shared" si="4"/>
-        <v>106372</v>
+        <v>106373</v>
       </c>
       <c r="C169">
         <v>232</v>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="B170">
         <f t="shared" si="4"/>
-        <v>106670</v>
+        <v>106671</v>
       </c>
       <c r="C170">
         <v>298</v>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="B171">
         <f t="shared" si="4"/>
-        <v>106914</v>
+        <v>106915</v>
       </c>
       <c r="C171">
         <v>244</v>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="B172">
         <f t="shared" si="4"/>
-        <v>107141</v>
+        <v>107142</v>
       </c>
       <c r="C172">
         <v>227</v>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="B173">
         <f t="shared" si="4"/>
-        <v>107269</v>
+        <v>107270</v>
       </c>
       <c r="C173">
         <v>128</v>
@@ -3648,7 +3648,7 @@
       </c>
       <c r="B174">
         <f t="shared" si="4"/>
-        <v>107343</v>
+        <v>107344</v>
       </c>
       <c r="C174">
         <v>74</v>
@@ -3664,7 +3664,7 @@
       </c>
       <c r="B175">
         <f t="shared" si="4"/>
-        <v>107622</v>
+        <v>107623</v>
       </c>
       <c r="C175">
         <v>279</v>
@@ -3680,7 +3680,7 @@
       </c>
       <c r="B176">
         <f t="shared" si="4"/>
-        <v>107877</v>
+        <v>107878</v>
       </c>
       <c r="C176">
         <v>255</v>
@@ -3696,7 +3696,7 @@
       </c>
       <c r="B177">
         <f t="shared" si="4"/>
-        <v>108135</v>
+        <v>108136</v>
       </c>
       <c r="C177">
         <v>258</v>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="B178">
         <f t="shared" si="4"/>
-        <v>108393</v>
+        <v>108394</v>
       </c>
       <c r="C178">
         <v>258</v>
@@ -3731,11 +3731,11 @@
         <v>108651</v>
       </c>
       <c r="C179">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D179">
         <f t="shared" si="5"/>
-        <v>215.71428571428572</v>
+        <v>215.57142857142858</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="D180">
         <f t="shared" si="5"/>
-        <v>220.14285714285714</v>
+        <v>220</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -3767,7 +3767,7 @@
       </c>
       <c r="D181">
         <f t="shared" si="5"/>
-        <v>224</v>
+        <v>223.85714285714286</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D182">
         <f t="shared" si="5"/>
-        <v>235.71428571428572</v>
+        <v>235.57142857142858</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -3799,7 +3799,7 @@
       </c>
       <c r="D183">
         <f t="shared" si="5"/>
-        <v>245</v>
+        <v>244.85714285714286</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -3815,7 +3815,7 @@
       </c>
       <c r="D184">
         <f t="shared" si="5"/>
-        <v>253.71428571428572</v>
+        <v>253.57142857142858</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
@@ -3831,7 +3831,7 @@
       </c>
       <c r="D185">
         <f t="shared" si="5"/>
-        <v>264.85714285714283</v>
+        <v>264.71428571428572</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -4464,14 +4464,14 @@
       </c>
       <c r="B225">
         <f t="shared" si="6"/>
-        <v>121839</v>
+        <v>121840</v>
       </c>
       <c r="C225">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D225">
         <f t="shared" si="7"/>
-        <v>316.14285714285717</v>
+        <v>316.28571428571428</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
@@ -4480,14 +4480,14 @@
       </c>
       <c r="B226">
         <f t="shared" si="6"/>
-        <v>122313</v>
+        <v>122314</v>
       </c>
       <c r="C226">
         <v>474</v>
       </c>
       <c r="D226">
         <f t="shared" si="7"/>
-        <v>329</v>
+        <v>329.14285714285717</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
@@ -4499,7 +4499,7 @@
         <v>122723</v>
       </c>
       <c r="C227">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D227">
         <f t="shared" si="7"/>
@@ -4583,7 +4583,7 @@
       </c>
       <c r="D232">
         <f t="shared" si="7"/>
-        <v>367</v>
+        <v>366.85714285714283</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
@@ -4599,7 +4599,7 @@
       </c>
       <c r="D233">
         <f t="shared" si="7"/>
-        <v>358.42857142857144</v>
+        <v>358.28571428571428</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
@@ -4800,14 +4800,14 @@
       </c>
       <c r="B246">
         <f t="shared" si="6"/>
-        <v>130774</v>
+        <v>130775</v>
       </c>
       <c r="C246">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="D246">
         <f t="shared" si="7"/>
-        <v>554.71428571428567</v>
+        <v>554.85714285714289</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
@@ -4816,14 +4816,14 @@
       </c>
       <c r="B247">
         <f t="shared" si="6"/>
-        <v>131387</v>
+        <v>131388</v>
       </c>
       <c r="C247">
         <v>613</v>
       </c>
       <c r="D247">
         <f t="shared" si="7"/>
-        <v>562.28571428571433</v>
+        <v>562.42857142857144</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
@@ -4832,14 +4832,14 @@
       </c>
       <c r="B248">
         <f t="shared" si="6"/>
-        <v>132070</v>
+        <v>132071</v>
       </c>
       <c r="C248">
         <v>683</v>
       </c>
       <c r="D248">
         <f t="shared" si="7"/>
-        <v>574.57142857142856</v>
+        <v>574.71428571428567</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
@@ -4848,14 +4848,14 @@
       </c>
       <c r="B249">
         <f t="shared" si="6"/>
-        <v>132635</v>
+        <v>132636</v>
       </c>
       <c r="C249">
         <v>565</v>
       </c>
       <c r="D249">
         <f t="shared" si="7"/>
-        <v>576.28571428571433</v>
+        <v>576.42857142857144</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
@@ -4864,14 +4864,14 @@
       </c>
       <c r="B250">
         <f t="shared" si="6"/>
-        <v>133043</v>
+        <v>133044</v>
       </c>
       <c r="C250">
         <v>408</v>
       </c>
       <c r="D250">
         <f t="shared" si="7"/>
-        <v>582.71428571428567</v>
+        <v>582.85714285714289</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
@@ -4880,14 +4880,14 @@
       </c>
       <c r="B251">
         <f t="shared" si="6"/>
-        <v>133335</v>
+        <v>133336</v>
       </c>
       <c r="C251">
         <v>292</v>
       </c>
       <c r="D251">
         <f t="shared" si="7"/>
-        <v>592.42857142857144</v>
+        <v>592.57142857142856</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
@@ -4896,14 +4896,14 @@
       </c>
       <c r="B252">
         <f t="shared" si="6"/>
-        <v>134086</v>
+        <v>134087</v>
       </c>
       <c r="C252">
         <v>751</v>
       </c>
       <c r="D252">
         <f t="shared" si="7"/>
-        <v>575.85714285714289</v>
+        <v>576</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="B253">
         <f t="shared" si="6"/>
-        <v>134820</v>
+        <v>134821</v>
       </c>
       <c r="C253">
         <v>734</v>
@@ -4928,7 +4928,7 @@
       </c>
       <c r="B254">
         <f t="shared" si="6"/>
-        <v>135539</v>
+        <v>135540</v>
       </c>
       <c r="C254">
         <v>719</v>
@@ -4944,14 +4944,14 @@
       </c>
       <c r="B255">
         <f t="shared" si="6"/>
-        <v>136372</v>
+        <v>136374</v>
       </c>
       <c r="C255">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="D255">
         <f t="shared" si="7"/>
-        <v>614.57142857142856</v>
+        <v>614.71428571428567</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
@@ -4960,14 +4960,14 @@
       </c>
       <c r="B256">
         <f t="shared" si="6"/>
-        <v>137062</v>
+        <v>137064</v>
       </c>
       <c r="C256">
         <v>690</v>
       </c>
       <c r="D256">
         <f t="shared" si="7"/>
-        <v>632.42857142857144</v>
+        <v>632.57142857142856</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.3">
@@ -4976,14 +4976,14 @@
       </c>
       <c r="B257">
         <f t="shared" si="6"/>
-        <v>137475</v>
+        <v>137477</v>
       </c>
       <c r="C257">
         <v>413</v>
       </c>
       <c r="D257">
         <f t="shared" si="7"/>
-        <v>633.14285714285711</v>
+        <v>633.28571428571433</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
@@ -4992,14 +4992,14 @@
       </c>
       <c r="B258">
         <f t="shared" si="6"/>
-        <v>137739</v>
+        <v>137741</v>
       </c>
       <c r="C258">
         <v>264</v>
       </c>
       <c r="D258">
         <f t="shared" si="7"/>
-        <v>629.14285714285711</v>
+        <v>629.28571428571433</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.3">
@@ -5008,14 +5008,14 @@
       </c>
       <c r="B259">
         <f t="shared" si="6"/>
-        <v>138332</v>
+        <v>138334</v>
       </c>
       <c r="C259">
         <v>593</v>
       </c>
       <c r="D259">
         <f t="shared" si="7"/>
-        <v>606.57142857142856</v>
+        <v>606.71428571428567</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
@@ -5024,14 +5024,14 @@
       </c>
       <c r="B260">
         <f t="shared" ref="B260:B286" si="8">C260+B259</f>
-        <v>139118</v>
+        <v>139120</v>
       </c>
       <c r="C260">
         <v>786</v>
       </c>
       <c r="D260">
         <f t="shared" si="7"/>
-        <v>614</v>
+        <v>614.14285714285711</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.3">
@@ -5040,14 +5040,14 @@
       </c>
       <c r="B261">
         <f t="shared" si="8"/>
-        <v>140016</v>
+        <v>140019</v>
       </c>
       <c r="C261">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D261">
         <f t="shared" si="7"/>
-        <v>639.57142857142856</v>
+        <v>639.85714285714289</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
@@ -5056,14 +5056,14 @@
       </c>
       <c r="B262">
         <f t="shared" si="8"/>
-        <v>140966</v>
+        <v>140969</v>
       </c>
       <c r="C262">
         <v>950</v>
       </c>
       <c r="D262">
         <f t="shared" si="7"/>
-        <v>656.28571428571433</v>
+        <v>656.42857142857144</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
@@ -5072,14 +5072,14 @@
       </c>
       <c r="B263">
         <f t="shared" si="8"/>
-        <v>141832</v>
+        <v>141835</v>
       </c>
       <c r="C263">
         <v>866</v>
       </c>
       <c r="D263">
         <f t="shared" si="7"/>
-        <v>681.42857142857144</v>
+        <v>681.57142857142856</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
@@ -5088,14 +5088,14 @@
       </c>
       <c r="B264">
         <f t="shared" si="8"/>
-        <v>142376</v>
+        <v>142379</v>
       </c>
       <c r="C264">
         <v>544</v>
       </c>
       <c r="D264">
         <f t="shared" si="7"/>
-        <v>700.14285714285711</v>
+        <v>700.28571428571433</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
@@ -5104,14 +5104,14 @@
       </c>
       <c r="B265">
         <f t="shared" si="8"/>
-        <v>142707</v>
+        <v>142710</v>
       </c>
       <c r="C265">
         <v>331</v>
       </c>
       <c r="D265">
         <f>AVERAGE(C259:C265)</f>
-        <v>709.71428571428567</v>
+        <v>709.85714285714289</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
@@ -5120,14 +5120,14 @@
       </c>
       <c r="B266">
         <f t="shared" si="8"/>
-        <v>143786</v>
+        <v>143789</v>
       </c>
       <c r="C266">
         <v>1079</v>
       </c>
       <c r="D266">
         <f t="shared" ref="D266:D279" si="9">AVERAGE(C260:C266)</f>
-        <v>779.14285714285711</v>
+        <v>779.28571428571433</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
@@ -5136,14 +5136,14 @@
       </c>
       <c r="B267">
         <f t="shared" si="8"/>
-        <v>144904</v>
+        <v>144907</v>
       </c>
       <c r="C267">
         <v>1118</v>
       </c>
       <c r="D267">
         <f t="shared" si="9"/>
-        <v>826.57142857142856</v>
+        <v>826.71428571428567</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="B268">
         <f t="shared" si="8"/>
-        <v>146106</v>
+        <v>146109</v>
       </c>
       <c r="C268">
         <v>1202</v>
@@ -5168,14 +5168,14 @@
       </c>
       <c r="B269">
         <f t="shared" si="8"/>
-        <v>147481</v>
+        <v>147483</v>
       </c>
       <c r="C269">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D269">
         <f t="shared" si="9"/>
-        <v>930.71428571428567</v>
+        <v>930.57142857142856</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
@@ -5184,14 +5184,14 @@
       </c>
       <c r="B270">
         <f t="shared" si="8"/>
-        <v>148706</v>
+        <v>148708</v>
       </c>
       <c r="C270">
         <v>1225</v>
       </c>
       <c r="D270">
         <f t="shared" si="9"/>
-        <v>982</v>
+        <v>981.85714285714289</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
@@ -5200,14 +5200,14 @@
       </c>
       <c r="B271">
         <f t="shared" si="8"/>
-        <v>149494</v>
+        <v>149496</v>
       </c>
       <c r="C271">
         <v>788</v>
       </c>
       <c r="D271">
         <f t="shared" si="9"/>
-        <v>1016.8571428571429</v>
+        <v>1016.7142857142857</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
@@ -5216,14 +5216,14 @@
       </c>
       <c r="B272">
         <f t="shared" si="8"/>
-        <v>149978</v>
+        <v>149980</v>
       </c>
       <c r="C272">
         <v>484</v>
       </c>
       <c r="D272">
         <f t="shared" si="9"/>
-        <v>1038.7142857142858</v>
+        <v>1038.5714285714287</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
@@ -5232,14 +5232,14 @@
       </c>
       <c r="B273">
         <f t="shared" si="8"/>
-        <v>151503</v>
+        <v>151505</v>
       </c>
       <c r="C273">
         <v>1525</v>
       </c>
       <c r="D273">
         <f t="shared" si="9"/>
-        <v>1102.4285714285713</v>
+        <v>1102.2857142857142</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.3">
@@ -5248,14 +5248,14 @@
       </c>
       <c r="B274">
         <f t="shared" si="8"/>
-        <v>152848</v>
+        <v>152850</v>
       </c>
       <c r="C274">
         <v>1345</v>
       </c>
       <c r="D274">
         <f t="shared" si="9"/>
-        <v>1134.8571428571429</v>
+        <v>1134.7142857142858</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
@@ -5264,14 +5264,14 @@
       </c>
       <c r="B275">
         <f t="shared" si="8"/>
-        <v>154289</v>
+        <v>154291</v>
       </c>
       <c r="C275">
         <v>1441</v>
       </c>
       <c r="D275">
         <f t="shared" si="9"/>
-        <v>1169</v>
+        <v>1168.8571428571429</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.3">
@@ -5280,7 +5280,7 @@
       </c>
       <c r="B276">
         <f t="shared" si="8"/>
-        <v>155673</v>
+        <v>155675</v>
       </c>
       <c r="C276">
         <v>1384</v>
@@ -5296,7 +5296,7 @@
       </c>
       <c r="B277">
         <f t="shared" si="8"/>
-        <v>156797</v>
+        <v>156799</v>
       </c>
       <c r="C277">
         <v>1124</v>
@@ -5312,7 +5312,7 @@
       </c>
       <c r="B278">
         <f t="shared" si="8"/>
-        <v>157668</v>
+        <v>157670</v>
       </c>
       <c r="C278">
         <v>871</v>
@@ -5328,7 +5328,7 @@
       </c>
       <c r="B279">
         <f t="shared" si="8"/>
-        <v>158190</v>
+        <v>158192</v>
       </c>
       <c r="C279">
         <v>522</v>
@@ -5344,13 +5344,13 @@
       </c>
       <c r="B280">
         <f t="shared" si="8"/>
-        <v>160027</v>
+        <v>160029</v>
       </c>
       <c r="C280">
         <v>1837</v>
       </c>
       <c r="D280">
-        <f t="shared" ref="D280:D316" si="10">AVERAGE(C274:C280)</f>
+        <f t="shared" ref="D280:D317" si="10">AVERAGE(C274:C280)</f>
         <v>1217.7142857142858</v>
       </c>
     </row>
@@ -5360,7 +5360,7 @@
       </c>
       <c r="B281">
         <f t="shared" si="8"/>
-        <v>161934</v>
+        <v>161936</v>
       </c>
       <c r="C281">
         <v>1907</v>
@@ -5376,7 +5376,7 @@
       </c>
       <c r="B282">
         <f t="shared" si="8"/>
-        <v>164111</v>
+        <v>164113</v>
       </c>
       <c r="C282">
         <v>2177</v>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="B283">
         <f t="shared" si="8"/>
-        <v>166530</v>
+        <v>166532</v>
       </c>
       <c r="C283">
         <v>2419</v>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="B284">
         <f t="shared" si="8"/>
-        <v>168769</v>
+        <v>168771</v>
       </c>
       <c r="C284">
         <v>2239</v>
@@ -5424,7 +5424,7 @@
       </c>
       <c r="B285">
         <f t="shared" si="8"/>
-        <v>170095</v>
+        <v>170097</v>
       </c>
       <c r="C285">
         <v>1326</v>
@@ -5440,7 +5440,7 @@
       </c>
       <c r="B286">
         <f t="shared" si="8"/>
-        <v>171038</v>
+        <v>171040</v>
       </c>
       <c r="C286">
         <v>943</v>
@@ -5455,8 +5455,8 @@
         <v>44144</v>
       </c>
       <c r="B287">
-        <f t="shared" ref="B287:B316" si="11">C287+B286</f>
-        <v>174215</v>
+        <f t="shared" ref="B287:B317" si="11">C287+B286</f>
+        <v>174217</v>
       </c>
       <c r="C287">
         <v>3177</v>
@@ -5472,7 +5472,7 @@
       </c>
       <c r="B288">
         <f t="shared" si="11"/>
-        <v>177035</v>
+        <v>177037</v>
       </c>
       <c r="C288">
         <v>2820</v>
@@ -5488,7 +5488,7 @@
       </c>
       <c r="B289">
         <f t="shared" si="11"/>
-        <v>179699</v>
+        <v>179701</v>
       </c>
       <c r="C289">
         <v>2664</v>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="B290">
         <f t="shared" si="11"/>
-        <v>182687</v>
+        <v>182689</v>
       </c>
       <c r="C290">
         <v>2988</v>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="B291">
         <f t="shared" si="11"/>
-        <v>185293</v>
+        <v>185295</v>
       </c>
       <c r="C291">
         <v>2606</v>
@@ -5536,7 +5536,7 @@
       </c>
       <c r="B292">
         <f t="shared" si="11"/>
-        <v>187005</v>
+        <v>187007</v>
       </c>
       <c r="C292">
         <v>1712</v>
@@ -5552,7 +5552,7 @@
       </c>
       <c r="B293">
         <f t="shared" si="11"/>
-        <v>188198</v>
+        <v>188200</v>
       </c>
       <c r="C293">
         <v>1193</v>
@@ -5568,14 +5568,14 @@
       </c>
       <c r="B294">
         <f t="shared" si="11"/>
-        <v>191716</v>
+        <v>191721</v>
       </c>
       <c r="C294">
-        <v>3518</v>
+        <v>3521</v>
       </c>
       <c r="D294">
         <f>AVERAGE(C288:C294)</f>
-        <v>2500.1428571428573</v>
+        <v>2500.5714285714284</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.3">
@@ -5584,14 +5584,14 @@
       </c>
       <c r="B295">
         <f t="shared" si="11"/>
-        <v>194849</v>
+        <v>194855</v>
       </c>
       <c r="C295">
-        <v>3133</v>
+        <v>3134</v>
       </c>
       <c r="D295">
         <f t="shared" si="10"/>
-        <v>2544.8571428571427</v>
+        <v>2545.4285714285716</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.3">
@@ -5600,14 +5600,14 @@
       </c>
       <c r="B296">
         <f t="shared" si="11"/>
-        <v>197765</v>
+        <v>197774</v>
       </c>
       <c r="C296">
-        <v>2916</v>
+        <v>2919</v>
       </c>
       <c r="D296">
         <f t="shared" si="10"/>
-        <v>2580.8571428571427</v>
+        <v>2581.8571428571427</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.3">
@@ -5616,14 +5616,14 @@
       </c>
       <c r="B297">
         <f t="shared" si="11"/>
-        <v>200760</v>
+        <v>200771</v>
       </c>
       <c r="C297">
-        <v>2995</v>
+        <v>2997</v>
       </c>
       <c r="D297">
         <f t="shared" si="10"/>
-        <v>2581.8571428571427</v>
+        <v>2583.1428571428573</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.3">
@@ -5632,14 +5632,14 @@
       </c>
       <c r="B298">
         <f t="shared" si="11"/>
-        <v>203613</v>
+        <v>203625</v>
       </c>
       <c r="C298">
-        <v>2853</v>
+        <v>2854</v>
       </c>
       <c r="D298">
         <f t="shared" si="10"/>
-        <v>2617.1428571428573</v>
+        <v>2618.5714285714284</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.3">
@@ -5648,14 +5648,14 @@
       </c>
       <c r="B299">
         <f t="shared" si="11"/>
-        <v>205380</v>
+        <v>205392</v>
       </c>
       <c r="C299">
         <v>1767</v>
       </c>
       <c r="D299">
         <f t="shared" si="10"/>
-        <v>2625</v>
+        <v>2626.4285714285716</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.3">
@@ -5664,14 +5664,14 @@
       </c>
       <c r="B300">
         <f t="shared" si="11"/>
-        <v>206568</v>
+        <v>206579</v>
       </c>
       <c r="C300">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="D300">
         <f t="shared" si="10"/>
-        <v>2624.2857142857142</v>
+        <v>2625.5714285714284</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.3">
@@ -5680,14 +5680,14 @@
       </c>
       <c r="B301">
         <f t="shared" si="11"/>
-        <v>210158</v>
+        <v>210169</v>
       </c>
       <c r="C301">
         <v>3590</v>
       </c>
       <c r="D301">
         <f t="shared" si="10"/>
-        <v>2634.5714285714284</v>
+        <v>2635.4285714285716</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.3">
@@ -5696,14 +5696,14 @@
       </c>
       <c r="B302">
         <f t="shared" si="11"/>
-        <v>213944</v>
+        <v>213958</v>
       </c>
       <c r="C302">
-        <v>3786</v>
+        <v>3789</v>
       </c>
       <c r="D302">
         <f t="shared" si="10"/>
-        <v>2727.8571428571427</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.3">
@@ -5712,14 +5712,14 @@
       </c>
       <c r="B303">
         <f t="shared" si="11"/>
-        <v>216882</v>
+        <v>216896</v>
       </c>
       <c r="C303">
         <v>2938</v>
       </c>
       <c r="D303">
         <f t="shared" si="10"/>
-        <v>2731</v>
+        <v>2731.7142857142858</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.3">
@@ -5728,14 +5728,14 @@
       </c>
       <c r="B304">
         <f t="shared" si="11"/>
-        <v>217329</v>
+        <v>217343</v>
       </c>
       <c r="C304">
         <v>447</v>
       </c>
       <c r="D304">
         <f t="shared" si="10"/>
-        <v>2367</v>
+        <v>2367.4285714285716</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
@@ -5744,14 +5744,14 @@
       </c>
       <c r="B305">
         <f t="shared" si="11"/>
-        <v>220689</v>
+        <v>220706</v>
       </c>
       <c r="C305">
-        <v>3360</v>
+        <v>3363</v>
       </c>
       <c r="D305">
         <f t="shared" si="10"/>
-        <v>2439.4285714285716</v>
+        <v>2440.1428571428573</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
@@ -5760,14 +5760,14 @@
       </c>
       <c r="B306">
         <f t="shared" si="11"/>
-        <v>223594</v>
+        <v>223611</v>
       </c>
       <c r="C306">
         <v>2905</v>
       </c>
       <c r="D306">
         <f t="shared" si="10"/>
-        <v>2602</v>
+        <v>2602.7142857142858</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
@@ -5776,14 +5776,14 @@
       </c>
       <c r="B307">
         <f t="shared" si="11"/>
-        <v>225346</v>
+        <v>225363</v>
       </c>
       <c r="C307">
         <v>1752</v>
       </c>
       <c r="D307">
         <f t="shared" si="10"/>
-        <v>2682.5714285714284</v>
+        <v>2683.4285714285716</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
@@ -5792,14 +5792,14 @@
       </c>
       <c r="B308">
         <f t="shared" si="11"/>
-        <v>230811</v>
+        <v>230840</v>
       </c>
       <c r="C308">
-        <v>5465</v>
+        <v>5477</v>
       </c>
       <c r="D308">
         <f t="shared" si="10"/>
-        <v>2950.4285714285716</v>
+        <v>2953</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.3">
@@ -5808,14 +5808,14 @@
       </c>
       <c r="B309">
         <f t="shared" si="11"/>
-        <v>236617</v>
+        <v>236674</v>
       </c>
       <c r="C309">
-        <v>5806</v>
+        <v>5834</v>
       </c>
       <c r="D309">
         <f t="shared" si="10"/>
-        <v>3239</v>
+        <v>3245.1428571428573</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.3">
@@ -5824,14 +5824,14 @@
       </c>
       <c r="B310">
         <f t="shared" si="11"/>
-        <v>242565</v>
+        <v>242699</v>
       </c>
       <c r="C310">
-        <v>5948</v>
+        <v>6025</v>
       </c>
       <c r="D310">
         <f t="shared" si="10"/>
-        <v>3669</v>
+        <v>3686.1428571428573</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.3">
@@ -5840,14 +5840,14 @@
       </c>
       <c r="B311">
         <f t="shared" si="11"/>
-        <v>247947</v>
+        <v>248321</v>
       </c>
       <c r="C311">
-        <v>5382</v>
+        <v>5622</v>
       </c>
       <c r="D311">
         <f t="shared" si="10"/>
-        <v>4374</v>
+        <v>4425.4285714285716</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
@@ -5856,14 +5856,14 @@
       </c>
       <c r="B312">
         <f t="shared" si="11"/>
-        <v>252527</v>
+        <v>253319</v>
       </c>
       <c r="C312">
-        <v>4580</v>
+        <v>4998</v>
       </c>
       <c r="D312">
         <f t="shared" si="10"/>
-        <v>4548.2857142857147</v>
+        <v>4659</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.3">
@@ -5872,14 +5872,14 @@
       </c>
       <c r="B313">
         <f t="shared" si="11"/>
-        <v>254169</v>
+        <v>255178</v>
       </c>
       <c r="C313">
-        <v>1642</v>
+        <v>1859</v>
       </c>
       <c r="D313">
         <f t="shared" si="10"/>
-        <v>4367.8571428571431</v>
+        <v>4509.5714285714284</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.3">
@@ -5888,14 +5888,14 @@
       </c>
       <c r="B314">
         <f t="shared" si="11"/>
-        <v>255493</v>
+        <v>256789</v>
       </c>
       <c r="C314">
-        <v>1324</v>
+        <v>1611</v>
       </c>
       <c r="D314">
         <f t="shared" si="10"/>
-        <v>4306.7142857142853</v>
+        <v>4489.4285714285716</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
@@ -5904,14 +5904,14 @@
       </c>
       <c r="B315">
         <f t="shared" si="11"/>
-        <v>259100</v>
+        <v>261159</v>
       </c>
       <c r="C315">
-        <v>3607</v>
+        <v>4370</v>
       </c>
       <c r="D315">
         <f t="shared" si="10"/>
-        <v>4041.2857142857142</v>
+        <v>4331.2857142857147</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.3">
@@ -5920,14 +5920,30 @@
       </c>
       <c r="B316">
         <f t="shared" si="11"/>
-        <v>259324</v>
+        <v>264211</v>
       </c>
       <c r="C316">
-        <v>224</v>
+        <v>3052</v>
       </c>
       <c r="D316">
         <f t="shared" si="10"/>
-        <v>3243.8571428571427</v>
+        <v>3933.8571428571427</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A317" s="1">
+        <v>44174</v>
+      </c>
+      <c r="B317">
+        <f t="shared" si="11"/>
+        <v>264454</v>
+      </c>
+      <c r="C317">
+        <v>243</v>
+      </c>
+      <c r="D317">
+        <f t="shared" si="10"/>
+        <v>3107.8571428571427</v>
       </c>
     </row>
   </sheetData>
@@ -5936,6 +5952,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5944,7 +5966,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008004546134034441816F24C41F65E929" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c3392cbe151f976ef883c2eee1f53348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0967b7be50301903c78f9c39c6fd9af8">
     <xsd:element name="properties">
@@ -6058,13 +6080,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E2A907-BC75-4262-BBD0-4F1B2976CD82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C76A581D-70D9-4324-B3C2-C549CBC3A500}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -6072,7 +6097,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A7812BB-980B-4585-92C6-973734300155}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6086,13 +6111,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E2A907-BC75-4262-BBD0-4F1B2976CD82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Today's update - 13Dec
</commit_message>
<xml_diff>
--- a/data/CasesByDate.xlsx
+++ b/data/CasesByDate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\COVID-19 Data Visualization\COVID19 - Files\Power BI resources\CSV filesPROB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D55BFE-8B82-4D00-B46B-40352F2055EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934032AC-9EA6-4C27-886A-3AFD330ED260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,13 +884,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D318"/>
+  <dimension ref="A1:D320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B308" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B290" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:C318"/>
+      <selection pane="bottomRight" activeCell="H315" sqref="H315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5350,7 +5350,7 @@
         <v>1837</v>
       </c>
       <c r="D280">
-        <f t="shared" ref="D280:D318" si="10">AVERAGE(C274:C280)</f>
+        <f t="shared" ref="D280:D320" si="10">AVERAGE(C274:C280)</f>
         <v>1217.8571428571429</v>
       </c>
     </row>
@@ -5455,7 +5455,7 @@
         <v>44144</v>
       </c>
       <c r="B287">
-        <f t="shared" ref="B287:B318" si="11">C287+B286</f>
+        <f t="shared" ref="B287:B319" si="11">C287+B286</f>
         <v>174218</v>
       </c>
       <c r="C287">
@@ -5504,14 +5504,14 @@
       </c>
       <c r="B290">
         <f t="shared" si="11"/>
-        <v>182690</v>
+        <v>182691</v>
       </c>
       <c r="C290">
-        <v>2988</v>
+        <v>2989</v>
       </c>
       <c r="D290">
         <f t="shared" si="10"/>
-        <v>2308.1428571428573</v>
+        <v>2308.2857142857142</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.3">
@@ -5520,14 +5520,14 @@
       </c>
       <c r="B291">
         <f t="shared" si="11"/>
-        <v>185296</v>
+        <v>185299</v>
       </c>
       <c r="C291">
-        <v>2606</v>
+        <v>2608</v>
       </c>
       <c r="D291">
         <f t="shared" si="10"/>
-        <v>2360.5714285714284</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.3">
@@ -5536,14 +5536,14 @@
       </c>
       <c r="B292">
         <f t="shared" si="11"/>
-        <v>187008</v>
+        <v>187011</v>
       </c>
       <c r="C292">
         <v>1712</v>
       </c>
       <c r="D292">
         <f t="shared" si="10"/>
-        <v>2415.7142857142858</v>
+        <v>2416.1428571428573</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.3">
@@ -5552,14 +5552,14 @@
       </c>
       <c r="B293">
         <f t="shared" si="11"/>
-        <v>188201</v>
+        <v>188204</v>
       </c>
       <c r="C293">
         <v>1193</v>
       </c>
       <c r="D293">
         <f t="shared" si="10"/>
-        <v>2451.4285714285716</v>
+        <v>2451.8571428571427</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.3">
@@ -5568,14 +5568,14 @@
       </c>
       <c r="B294">
         <f t="shared" si="11"/>
-        <v>191723</v>
+        <v>191726</v>
       </c>
       <c r="C294">
         <v>3522</v>
       </c>
       <c r="D294">
         <f>AVERAGE(C288:C294)</f>
-        <v>2500.7142857142858</v>
+        <v>2501.1428571428573</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.3">
@@ -5584,14 +5584,14 @@
       </c>
       <c r="B295">
         <f t="shared" si="11"/>
-        <v>194857</v>
+        <v>194861</v>
       </c>
       <c r="C295">
-        <v>3134</v>
+        <v>3135</v>
       </c>
       <c r="D295">
         <f t="shared" si="10"/>
-        <v>2545.5714285714284</v>
+        <v>2546.1428571428573</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.3">
@@ -5600,14 +5600,14 @@
       </c>
       <c r="B296">
         <f t="shared" si="11"/>
-        <v>197778</v>
+        <v>197784</v>
       </c>
       <c r="C296">
-        <v>2921</v>
+        <v>2923</v>
       </c>
       <c r="D296">
         <f t="shared" si="10"/>
-        <v>2582.2857142857142</v>
+        <v>2583.1428571428573</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.3">
@@ -5616,14 +5616,14 @@
       </c>
       <c r="B297">
         <f t="shared" si="11"/>
-        <v>200779</v>
+        <v>200785</v>
       </c>
       <c r="C297">
         <v>3001</v>
       </c>
       <c r="D297">
         <f t="shared" si="10"/>
-        <v>2584.1428571428573</v>
+        <v>2584.8571428571427</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.3">
@@ -5632,14 +5632,14 @@
       </c>
       <c r="B298">
         <f t="shared" si="11"/>
-        <v>203631</v>
+        <v>203635</v>
       </c>
       <c r="C298">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="D298">
         <f t="shared" si="10"/>
-        <v>2619.2857142857142</v>
+        <v>2619.4285714285716</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.3">
@@ -5648,14 +5648,14 @@
       </c>
       <c r="B299">
         <f t="shared" si="11"/>
-        <v>205398</v>
+        <v>205402</v>
       </c>
       <c r="C299">
         <v>1767</v>
       </c>
       <c r="D299">
         <f t="shared" si="10"/>
-        <v>2627.1428571428573</v>
+        <v>2627.2857142857142</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.3">
@@ -5664,14 +5664,14 @@
       </c>
       <c r="B300">
         <f t="shared" si="11"/>
-        <v>206585</v>
+        <v>206589</v>
       </c>
       <c r="C300">
         <v>1187</v>
       </c>
       <c r="D300">
         <f t="shared" si="10"/>
-        <v>2626.2857142857142</v>
+        <v>2626.4285714285716</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.3">
@@ -5680,14 +5680,14 @@
       </c>
       <c r="B301">
         <f t="shared" si="11"/>
-        <v>210175</v>
+        <v>210182</v>
       </c>
       <c r="C301">
-        <v>3590</v>
+        <v>3593</v>
       </c>
       <c r="D301">
         <f t="shared" si="10"/>
-        <v>2636</v>
+        <v>2636.5714285714284</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.3">
@@ -5696,14 +5696,14 @@
       </c>
       <c r="B302">
         <f t="shared" si="11"/>
-        <v>213965</v>
+        <v>213976</v>
       </c>
       <c r="C302">
-        <v>3790</v>
+        <v>3794</v>
       </c>
       <c r="D302">
         <f t="shared" si="10"/>
-        <v>2729.7142857142858</v>
+        <v>2730.7142857142858</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.3">
@@ -5712,14 +5712,14 @@
       </c>
       <c r="B303">
         <f t="shared" si="11"/>
-        <v>216906</v>
+        <v>216916</v>
       </c>
       <c r="C303">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="D303">
         <f t="shared" si="10"/>
-        <v>2732.5714285714284</v>
+        <v>2733.1428571428573</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.3">
@@ -5728,14 +5728,14 @@
       </c>
       <c r="B304">
         <f t="shared" si="11"/>
-        <v>217353</v>
+        <v>217362</v>
       </c>
       <c r="C304">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D304">
         <f t="shared" si="10"/>
-        <v>2367.7142857142858</v>
+        <v>2368.1428571428573</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
@@ -5744,14 +5744,14 @@
       </c>
       <c r="B305">
         <f t="shared" si="11"/>
-        <v>220716</v>
+        <v>220726</v>
       </c>
       <c r="C305">
-        <v>3363</v>
+        <v>3364</v>
       </c>
       <c r="D305">
         <f t="shared" si="10"/>
-        <v>2440.7142857142858</v>
+        <v>2441.5714285714284</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
@@ -5760,14 +5760,14 @@
       </c>
       <c r="B306">
         <f t="shared" si="11"/>
-        <v>223621</v>
+        <v>223629</v>
       </c>
       <c r="C306">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="D306">
         <f t="shared" si="10"/>
-        <v>2603.2857142857142</v>
+        <v>2603.8571428571427</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
@@ -5776,14 +5776,14 @@
       </c>
       <c r="B307">
         <f t="shared" si="11"/>
-        <v>225373</v>
+        <v>225382</v>
       </c>
       <c r="C307">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="D307">
         <f t="shared" si="10"/>
-        <v>2684</v>
+        <v>2684.7142857142858</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
@@ -5792,14 +5792,14 @@
       </c>
       <c r="B308">
         <f t="shared" si="11"/>
-        <v>230849</v>
+        <v>230866</v>
       </c>
       <c r="C308">
-        <v>5476</v>
+        <v>5484</v>
       </c>
       <c r="D308">
         <f t="shared" si="10"/>
-        <v>2953.4285714285716</v>
+        <v>2954.8571428571427</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.3">
@@ -5808,14 +5808,14 @@
       </c>
       <c r="B309">
         <f t="shared" si="11"/>
-        <v>236689</v>
+        <v>236708</v>
       </c>
       <c r="C309">
-        <v>5840</v>
+        <v>5842</v>
       </c>
       <c r="D309">
         <f t="shared" si="10"/>
-        <v>3246.2857142857142</v>
+        <v>3247.4285714285716</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.3">
@@ -5824,14 +5824,14 @@
       </c>
       <c r="B310">
         <f t="shared" si="11"/>
-        <v>242734</v>
+        <v>242759</v>
       </c>
       <c r="C310">
-        <v>6045</v>
+        <v>6051</v>
       </c>
       <c r="D310">
         <f t="shared" si="10"/>
-        <v>3689.7142857142858</v>
+        <v>3691.8571428571427</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.3">
@@ -5840,14 +5840,14 @@
       </c>
       <c r="B311">
         <f t="shared" si="11"/>
-        <v>248443</v>
+        <v>248499</v>
       </c>
       <c r="C311">
-        <v>5709</v>
+        <v>5740</v>
       </c>
       <c r="D311">
         <f t="shared" si="10"/>
-        <v>4441.4285714285716</v>
+        <v>4448.1428571428569</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
@@ -5856,14 +5856,14 @@
       </c>
       <c r="B312">
         <f t="shared" si="11"/>
-        <v>253643</v>
+        <v>253784</v>
       </c>
       <c r="C312">
-        <v>5200</v>
+        <v>5285</v>
       </c>
       <c r="D312">
         <f t="shared" si="10"/>
-        <v>4703.8571428571431</v>
+        <v>4722.5714285714284</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.3">
@@ -5872,14 +5872,14 @@
       </c>
       <c r="B313">
         <f t="shared" si="11"/>
-        <v>255687</v>
+        <v>255950</v>
       </c>
       <c r="C313">
-        <v>2044</v>
+        <v>2166</v>
       </c>
       <c r="D313">
         <f t="shared" si="10"/>
-        <v>4580.8571428571431</v>
+        <v>4617.2857142857147</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.3">
@@ -5888,14 +5888,14 @@
       </c>
       <c r="B314">
         <f t="shared" si="11"/>
-        <v>257656</v>
+        <v>258042</v>
       </c>
       <c r="C314">
-        <v>1969</v>
+        <v>2092</v>
       </c>
       <c r="D314">
         <f t="shared" si="10"/>
-        <v>4611.8571428571431</v>
+        <v>4665.7142857142853</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
@@ -5904,14 +5904,14 @@
       </c>
       <c r="B315">
         <f t="shared" si="11"/>
-        <v>262750</v>
+        <v>264077</v>
       </c>
       <c r="C315">
-        <v>5094</v>
+        <v>6035</v>
       </c>
       <c r="D315">
         <f t="shared" si="10"/>
-        <v>4557.2857142857147</v>
+        <v>4744.4285714285716</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.3">
@@ -5920,14 +5920,14 @@
       </c>
       <c r="B316">
         <f t="shared" si="11"/>
-        <v>266560</v>
+        <v>268995</v>
       </c>
       <c r="C316">
-        <v>3810</v>
+        <v>4918</v>
       </c>
       <c r="D316">
         <f t="shared" si="10"/>
-        <v>4267.2857142857147</v>
+        <v>4612.4285714285716</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.3">
@@ -5936,14 +5936,14 @@
       </c>
       <c r="B317">
         <f t="shared" si="11"/>
-        <v>269617</v>
+        <v>273126</v>
       </c>
       <c r="C317">
-        <v>3057</v>
+        <v>4131</v>
       </c>
       <c r="D317">
         <f t="shared" si="10"/>
-        <v>3840.4285714285716</v>
+        <v>4338.1428571428569</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.3">
@@ -5952,14 +5952,46 @@
       </c>
       <c r="B318">
         <f t="shared" si="11"/>
-        <v>269929</v>
+        <v>276766</v>
       </c>
       <c r="C318">
-        <v>312</v>
+        <v>3640</v>
       </c>
       <c r="D318">
         <f t="shared" si="10"/>
-        <v>3069.4285714285716</v>
+        <v>4038.1428571428573</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A319" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B319">
+        <f t="shared" si="11"/>
+        <v>279363</v>
+      </c>
+      <c r="C319">
+        <v>2597</v>
+      </c>
+      <c r="D319">
+        <f t="shared" si="10"/>
+        <v>3654.1428571428573</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A320" s="1">
+        <v>44177</v>
+      </c>
+      <c r="B320">
+        <f t="shared" ref="B320" si="12">C320+B319</f>
+        <v>279574</v>
+      </c>
+      <c r="C320">
+        <v>211</v>
+      </c>
+      <c r="D320">
+        <f t="shared" si="10"/>
+        <v>3374.8571428571427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
21 Dec - "This time for sure! Presto!!"
</commit_message>
<xml_diff>
--- a/data/CasesByDate.xlsx
+++ b/data/CasesByDate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\COVID-19 Data Visualization\COVID19 - Files\Power BI resources\CSV filesPROB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E116D2A-3C7C-4D43-80AE-9F8FF91DB9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0486FC7-B2AF-40BD-85E3-C7E1692FE97A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CasesByDate" sheetId="1" r:id="rId1"/>
@@ -884,13 +884,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D326"/>
+  <dimension ref="A1:D328"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B311" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B317" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="B337" sqref="B337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5136,14 +5136,14 @@
       </c>
       <c r="B267">
         <f t="shared" si="8"/>
-        <v>144890</v>
+        <v>144891</v>
       </c>
       <c r="C267">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="D267">
         <f t="shared" si="9"/>
-        <v>826.71428571428567</v>
+        <v>826.85714285714289</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
@@ -5152,14 +5152,14 @@
       </c>
       <c r="B268">
         <f t="shared" si="8"/>
-        <v>146091</v>
+        <v>146092</v>
       </c>
       <c r="C268">
         <v>1201</v>
       </c>
       <c r="D268">
         <f t="shared" si="9"/>
-        <v>869.85714285714289</v>
+        <v>870</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
@@ -5168,14 +5168,14 @@
       </c>
       <c r="B269">
         <f t="shared" si="8"/>
-        <v>147466</v>
+        <v>147467</v>
       </c>
       <c r="C269">
         <v>1375</v>
       </c>
       <c r="D269">
         <f t="shared" si="9"/>
-        <v>930.57142857142856</v>
+        <v>930.71428571428567</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
@@ -5184,14 +5184,14 @@
       </c>
       <c r="B270">
         <f t="shared" si="8"/>
-        <v>148691</v>
+        <v>148692</v>
       </c>
       <c r="C270">
         <v>1225</v>
       </c>
       <c r="D270">
         <f t="shared" si="9"/>
-        <v>981.85714285714289</v>
+        <v>982</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
@@ -5200,14 +5200,14 @@
       </c>
       <c r="B271">
         <f t="shared" si="8"/>
-        <v>149479</v>
+        <v>149480</v>
       </c>
       <c r="C271">
         <v>788</v>
       </c>
       <c r="D271">
         <f t="shared" si="9"/>
-        <v>1016.7142857142857</v>
+        <v>1016.8571428571429</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
@@ -5216,14 +5216,14 @@
       </c>
       <c r="B272">
         <f t="shared" si="8"/>
-        <v>149963</v>
+        <v>149964</v>
       </c>
       <c r="C272">
         <v>484</v>
       </c>
       <c r="D272">
         <f t="shared" si="9"/>
-        <v>1038.5714285714287</v>
+        <v>1038.7142857142858</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
@@ -5232,14 +5232,14 @@
       </c>
       <c r="B273">
         <f t="shared" si="8"/>
-        <v>151488</v>
+        <v>151489</v>
       </c>
       <c r="C273">
         <v>1525</v>
       </c>
       <c r="D273">
         <f t="shared" si="9"/>
-        <v>1102.2857142857142</v>
+        <v>1102.4285714285713</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.3">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="B274">
         <f t="shared" si="8"/>
-        <v>152833</v>
+        <v>152834</v>
       </c>
       <c r="C274">
         <v>1345</v>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="B275">
         <f t="shared" si="8"/>
-        <v>154273</v>
+        <v>154274</v>
       </c>
       <c r="C275">
         <v>1440</v>
@@ -5280,7 +5280,7 @@
       </c>
       <c r="B276">
         <f t="shared" si="8"/>
-        <v>155658</v>
+        <v>155659</v>
       </c>
       <c r="C276">
         <v>1385</v>
@@ -5296,7 +5296,7 @@
       </c>
       <c r="B277">
         <f t="shared" si="8"/>
-        <v>156782</v>
+        <v>156783</v>
       </c>
       <c r="C277">
         <v>1124</v>
@@ -5312,7 +5312,7 @@
       </c>
       <c r="B278">
         <f t="shared" si="8"/>
-        <v>157653</v>
+        <v>157654</v>
       </c>
       <c r="C278">
         <v>871</v>
@@ -5328,7 +5328,7 @@
       </c>
       <c r="B279">
         <f t="shared" si="8"/>
-        <v>158175</v>
+        <v>158176</v>
       </c>
       <c r="C279">
         <v>522</v>
@@ -5344,14 +5344,14 @@
       </c>
       <c r="B280">
         <f t="shared" si="8"/>
-        <v>160012</v>
+        <v>160014</v>
       </c>
       <c r="C280">
-        <v>1837</v>
+        <v>1838</v>
       </c>
       <c r="D280">
-        <f t="shared" ref="D280:D326" si="10">AVERAGE(C274:C280)</f>
-        <v>1217.7142857142858</v>
+        <f t="shared" ref="D280:D328" si="10">AVERAGE(C274:C280)</f>
+        <v>1217.8571428571429</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
@@ -5360,14 +5360,14 @@
       </c>
       <c r="B281">
         <f t="shared" si="8"/>
-        <v>161918</v>
+        <v>161920</v>
       </c>
       <c r="C281">
         <v>1906</v>
       </c>
       <c r="D281">
         <f t="shared" si="10"/>
-        <v>1297.8571428571429</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
@@ -5376,14 +5376,14 @@
       </c>
       <c r="B282">
         <f t="shared" si="8"/>
-        <v>164092</v>
+        <v>164094</v>
       </c>
       <c r="C282">
         <v>2174</v>
       </c>
       <c r="D282">
         <f t="shared" si="10"/>
-        <v>1402.7142857142858</v>
+        <v>1402.8571428571429</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.3">
@@ -5392,14 +5392,14 @@
       </c>
       <c r="B283">
         <f t="shared" si="8"/>
-        <v>166509</v>
+        <v>166511</v>
       </c>
       <c r="C283">
         <v>2417</v>
       </c>
       <c r="D283">
         <f t="shared" si="10"/>
-        <v>1550.1428571428571</v>
+        <v>1550.2857142857142</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.3">
@@ -5408,10 +5408,10 @@
       </c>
       <c r="B284">
         <f t="shared" si="8"/>
-        <v>168747</v>
+        <v>168748</v>
       </c>
       <c r="C284">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="D284">
         <f t="shared" si="10"/>
@@ -5424,7 +5424,7 @@
       </c>
       <c r="B285">
         <f t="shared" si="8"/>
-        <v>170073</v>
+        <v>170074</v>
       </c>
       <c r="C285">
         <v>1326</v>
@@ -5440,7 +5440,7 @@
       </c>
       <c r="B286">
         <f t="shared" si="8"/>
-        <v>171016</v>
+        <v>171017</v>
       </c>
       <c r="C286">
         <v>943</v>
@@ -5456,14 +5456,14 @@
       </c>
       <c r="B287">
         <f t="shared" ref="B287:B319" si="11">C287+B286</f>
-        <v>174193</v>
+        <v>174194</v>
       </c>
       <c r="C287">
         <v>3177</v>
       </c>
       <c r="D287">
         <f t="shared" si="10"/>
-        <v>2025.8571428571429</v>
+        <v>2025.7142857142858</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.3">
@@ -5472,14 +5472,14 @@
       </c>
       <c r="B288">
         <f t="shared" si="11"/>
-        <v>177011</v>
+        <v>177012</v>
       </c>
       <c r="C288">
         <v>2818</v>
       </c>
       <c r="D288">
         <f t="shared" si="10"/>
-        <v>2156.1428571428573</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.3">
@@ -5488,14 +5488,14 @@
       </c>
       <c r="B289">
         <f t="shared" si="11"/>
-        <v>179674</v>
+        <v>179675</v>
       </c>
       <c r="C289">
         <v>2663</v>
       </c>
       <c r="D289">
         <f t="shared" si="10"/>
-        <v>2226</v>
+        <v>2225.8571428571427</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.3">
@@ -5504,14 +5504,14 @@
       </c>
       <c r="B290">
         <f t="shared" si="11"/>
-        <v>182661</v>
+        <v>182662</v>
       </c>
       <c r="C290">
         <v>2987</v>
       </c>
       <c r="D290">
         <f t="shared" si="10"/>
-        <v>2307.4285714285716</v>
+        <v>2307.2857142857142</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.3">
@@ -5520,7 +5520,7 @@
       </c>
       <c r="B291">
         <f t="shared" si="11"/>
-        <v>185268</v>
+        <v>185269</v>
       </c>
       <c r="C291">
         <v>2607</v>
@@ -5536,7 +5536,7 @@
       </c>
       <c r="B292">
         <f t="shared" si="11"/>
-        <v>186978</v>
+        <v>186979</v>
       </c>
       <c r="C292">
         <v>1710</v>
@@ -5552,7 +5552,7 @@
       </c>
       <c r="B293">
         <f t="shared" si="11"/>
-        <v>188170</v>
+        <v>188171</v>
       </c>
       <c r="C293">
         <v>1192</v>
@@ -5568,14 +5568,14 @@
       </c>
       <c r="B294">
         <f t="shared" si="11"/>
-        <v>191694</v>
+        <v>191696</v>
       </c>
       <c r="C294">
-        <v>3524</v>
+        <v>3525</v>
       </c>
       <c r="D294">
         <f>AVERAGE(C288:C294)</f>
-        <v>2500.1428571428573</v>
+        <v>2500.2857142857142</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.3">
@@ -5584,10 +5584,10 @@
       </c>
       <c r="B295">
         <f t="shared" si="11"/>
-        <v>194828</v>
+        <v>194829</v>
       </c>
       <c r="C295">
-        <v>3134</v>
+        <v>3133</v>
       </c>
       <c r="D295">
         <f t="shared" si="10"/>
@@ -5600,7 +5600,7 @@
       </c>
       <c r="B296">
         <f t="shared" si="11"/>
-        <v>197751</v>
+        <v>197752</v>
       </c>
       <c r="C296">
         <v>2923</v>
@@ -5616,7 +5616,7 @@
       </c>
       <c r="B297">
         <f t="shared" si="11"/>
-        <v>200752</v>
+        <v>200753</v>
       </c>
       <c r="C297">
         <v>3001</v>
@@ -5632,7 +5632,7 @@
       </c>
       <c r="B298">
         <f t="shared" si="11"/>
-        <v>203599</v>
+        <v>203600</v>
       </c>
       <c r="C298">
         <v>2847</v>
@@ -5651,11 +5651,11 @@
         <v>205367</v>
       </c>
       <c r="C299">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="D299">
         <f t="shared" si="10"/>
-        <v>2627</v>
+        <v>2626.8571428571427</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.3">
@@ -5671,7 +5671,7 @@
       </c>
       <c r="D300">
         <f t="shared" si="10"/>
-        <v>2626.5714285714284</v>
+        <v>2626.4285714285716</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.3">
@@ -5687,7 +5687,7 @@
       </c>
       <c r="D301">
         <f t="shared" si="10"/>
-        <v>2636.8571428571427</v>
+        <v>2636.5714285714284</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.3">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="D302">
         <f t="shared" si="10"/>
-        <v>2730.8571428571427</v>
+        <v>2730.7142857142858</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.3">
@@ -5712,10 +5712,10 @@
       </c>
       <c r="B303">
         <f t="shared" si="11"/>
-        <v>216885</v>
+        <v>216886</v>
       </c>
       <c r="C303">
-        <v>2941</v>
+        <v>2942</v>
       </c>
       <c r="D303">
         <f t="shared" si="10"/>
@@ -5728,7 +5728,7 @@
       </c>
       <c r="B304">
         <f t="shared" si="11"/>
-        <v>217330</v>
+        <v>217331</v>
       </c>
       <c r="C304">
         <v>445</v>
@@ -5744,14 +5744,14 @@
       </c>
       <c r="B305">
         <f t="shared" si="11"/>
-        <v>220709</v>
+        <v>220711</v>
       </c>
       <c r="C305">
-        <v>3379</v>
+        <v>3380</v>
       </c>
       <c r="D305">
         <f t="shared" si="10"/>
-        <v>2444.2857142857142</v>
+        <v>2444.4285714285716</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
@@ -5760,14 +5760,14 @@
       </c>
       <c r="B306">
         <f t="shared" si="11"/>
-        <v>223612</v>
+        <v>223614</v>
       </c>
       <c r="C306">
         <v>2903</v>
       </c>
       <c r="D306">
         <f t="shared" si="10"/>
-        <v>2606.4285714285716</v>
+        <v>2606.7142857142858</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
@@ -5776,14 +5776,14 @@
       </c>
       <c r="B307">
         <f t="shared" si="11"/>
-        <v>225372</v>
+        <v>225374</v>
       </c>
       <c r="C307">
         <v>1760</v>
       </c>
       <c r="D307">
         <f t="shared" si="10"/>
-        <v>2688</v>
+        <v>2688.2857142857142</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
@@ -5792,14 +5792,14 @@
       </c>
       <c r="B308">
         <f t="shared" si="11"/>
-        <v>230873</v>
+        <v>230879</v>
       </c>
       <c r="C308">
-        <v>5501</v>
+        <v>5505</v>
       </c>
       <c r="D308">
         <f t="shared" si="10"/>
-        <v>2960.1428571428573</v>
+        <v>2961</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.3">
@@ -5808,14 +5808,14 @@
       </c>
       <c r="B309">
         <f t="shared" si="11"/>
-        <v>236727</v>
+        <v>236739</v>
       </c>
       <c r="C309">
-        <v>5854</v>
+        <v>5860</v>
       </c>
       <c r="D309">
         <f t="shared" si="10"/>
-        <v>3254.7142857142858</v>
+        <v>3256.4285714285716</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.3">
@@ -5824,14 +5824,14 @@
       </c>
       <c r="B310">
         <f t="shared" si="11"/>
-        <v>242794</v>
+        <v>242814</v>
       </c>
       <c r="C310">
-        <v>6067</v>
+        <v>6075</v>
       </c>
       <c r="D310">
         <f t="shared" si="10"/>
-        <v>3701.2857142857142</v>
+        <v>3704</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.3">
@@ -5840,14 +5840,14 @@
       </c>
       <c r="B311">
         <f t="shared" si="11"/>
-        <v>248541</v>
+        <v>248571</v>
       </c>
       <c r="C311">
-        <v>5747</v>
+        <v>5757</v>
       </c>
       <c r="D311">
         <f t="shared" si="10"/>
-        <v>4458.7142857142853</v>
+        <v>4462.8571428571431</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
@@ -5856,14 +5856,14 @@
       </c>
       <c r="B312">
         <f t="shared" si="11"/>
-        <v>253824</v>
+        <v>253854</v>
       </c>
       <c r="C312">
         <v>5283</v>
       </c>
       <c r="D312">
         <f t="shared" si="10"/>
-        <v>4730.7142857142853</v>
+        <v>4734.7142857142853</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.3">
@@ -5872,14 +5872,14 @@
       </c>
       <c r="B313">
         <f t="shared" si="11"/>
-        <v>256004</v>
+        <v>256034</v>
       </c>
       <c r="C313">
         <v>2180</v>
       </c>
       <c r="D313">
         <f t="shared" si="10"/>
-        <v>4627.4285714285716</v>
+        <v>4631.4285714285716</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.3">
@@ -5888,14 +5888,14 @@
       </c>
       <c r="B314">
         <f t="shared" si="11"/>
-        <v>258106</v>
+        <v>258135</v>
       </c>
       <c r="C314">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="D314">
         <f t="shared" si="10"/>
-        <v>4676.2857142857147</v>
+        <v>4680.1428571428569</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
@@ -5904,14 +5904,14 @@
       </c>
       <c r="B315">
         <f t="shared" si="11"/>
-        <v>264301</v>
+        <v>264334</v>
       </c>
       <c r="C315">
-        <v>6195</v>
+        <v>6199</v>
       </c>
       <c r="D315">
         <f t="shared" si="10"/>
-        <v>4775.4285714285716</v>
+        <v>4779.2857142857147</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.3">
@@ -5920,14 +5920,14 @@
       </c>
       <c r="B316">
         <f t="shared" si="11"/>
-        <v>269691</v>
+        <v>269731</v>
       </c>
       <c r="C316">
-        <v>5390</v>
+        <v>5397</v>
       </c>
       <c r="D316">
         <f t="shared" si="10"/>
-        <v>4709.1428571428569</v>
+        <v>4713.1428571428569</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.3">
@@ -5936,14 +5936,14 @@
       </c>
       <c r="B317">
         <f t="shared" si="11"/>
-        <v>275092</v>
+        <v>275131</v>
       </c>
       <c r="C317">
-        <v>5401</v>
+        <v>5400</v>
       </c>
       <c r="D317">
         <f t="shared" si="10"/>
-        <v>4614</v>
+        <v>4616.7142857142853</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.3">
@@ -5952,14 +5952,14 @@
       </c>
       <c r="B318">
         <f t="shared" si="11"/>
-        <v>280512</v>
+        <v>280570</v>
       </c>
       <c r="C318">
-        <v>5420</v>
+        <v>5439</v>
       </c>
       <c r="D318">
         <f t="shared" si="10"/>
-        <v>4567.2857142857147</v>
+        <v>4571.2857142857147</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.3">
@@ -5968,14 +5968,14 @@
       </c>
       <c r="B319">
         <f t="shared" si="11"/>
-        <v>285410</v>
+        <v>285470</v>
       </c>
       <c r="C319">
-        <v>4898</v>
+        <v>4900</v>
       </c>
       <c r="D319">
         <f t="shared" si="10"/>
-        <v>4512.2857142857147</v>
+        <v>4516.5714285714284</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.3">
@@ -5984,14 +5984,14 @@
       </c>
       <c r="B320">
         <f t="shared" ref="B320:B321" si="12">C320+B319</f>
-        <v>288217</v>
+        <v>288280</v>
       </c>
       <c r="C320">
-        <v>2807</v>
+        <v>2810</v>
       </c>
       <c r="D320">
         <f t="shared" si="10"/>
-        <v>4601.8571428571431</v>
+        <v>4606.5714285714284</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.3">
@@ -6000,14 +6000,14 @@
       </c>
       <c r="B321">
         <f t="shared" si="12"/>
-        <v>290359</v>
+        <v>290428</v>
       </c>
       <c r="C321">
-        <v>2142</v>
+        <v>2148</v>
       </c>
       <c r="D321">
         <f t="shared" si="10"/>
-        <v>4607.5714285714284</v>
+        <v>4613.2857142857147</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.3">
@@ -6016,14 +6016,14 @@
       </c>
       <c r="B322">
         <f t="shared" ref="B322:B324" si="13">C322+B321</f>
-        <v>296396</v>
+        <v>296594</v>
       </c>
       <c r="C322">
-        <v>6037</v>
+        <v>6166</v>
       </c>
       <c r="D322">
         <f t="shared" si="10"/>
-        <v>4585</v>
+        <v>4608.5714285714284</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.3">
@@ -6032,14 +6032,14 @@
       </c>
       <c r="B323">
         <f t="shared" si="13"/>
-        <v>301716</v>
+        <v>302418</v>
       </c>
       <c r="C323">
-        <v>5320</v>
+        <v>5824</v>
       </c>
       <c r="D323">
         <f t="shared" si="10"/>
-        <v>4575</v>
+        <v>4669.5714285714284</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.3">
@@ -6048,14 +6048,14 @@
       </c>
       <c r="B324">
         <f t="shared" si="13"/>
-        <v>305908</v>
+        <v>307661</v>
       </c>
       <c r="C324">
-        <v>4192</v>
+        <v>5243</v>
       </c>
       <c r="D324">
         <f t="shared" si="10"/>
-        <v>4402.2857142857147</v>
+        <v>4647.1428571428569</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.3">
@@ -6063,15 +6063,15 @@
         <v>44182</v>
       </c>
       <c r="B325">
-        <f t="shared" ref="B325:B326" si="14">C325+B324</f>
-        <v>306647</v>
+        <f t="shared" ref="B325:B328" si="14">C325+B324</f>
+        <v>308939</v>
       </c>
       <c r="C325">
-        <v>739</v>
+        <v>1278</v>
       </c>
       <c r="D325">
         <f t="shared" si="10"/>
-        <v>3733.5714285714284</v>
+        <v>4052.7142857142858</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.3">
@@ -6080,14 +6080,46 @@
       </c>
       <c r="B326">
         <f t="shared" si="14"/>
-        <v>306928</v>
+        <v>312773</v>
       </c>
       <c r="C326">
-        <v>281</v>
+        <v>3834</v>
       </c>
       <c r="D326">
         <f t="shared" si="10"/>
-        <v>3074</v>
+        <v>3900.4285714285716</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A327" s="1">
+        <v>44184</v>
+      </c>
+      <c r="B327">
+        <f t="shared" si="14"/>
+        <v>314724</v>
+      </c>
+      <c r="C327">
+        <v>1951</v>
+      </c>
+      <c r="D327">
+        <f t="shared" si="10"/>
+        <v>3777.7142857142858</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A328" s="1">
+        <v>44185</v>
+      </c>
+      <c r="B328">
+        <f t="shared" si="14"/>
+        <v>314850</v>
+      </c>
+      <c r="C328">
+        <v>126</v>
+      </c>
+      <c r="D328">
+        <f t="shared" si="10"/>
+        <v>3488.8571428571427</v>
       </c>
     </row>
   </sheetData>
@@ -6096,21 +6128,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008004546134034441816F24C41F65E929" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c3392cbe151f976ef883c2eee1f53348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0967b7be50301903c78f9c39c6fd9af8">
     <xsd:element name="properties">
@@ -6224,24 +6241,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E2A907-BC75-4262-BBD0-4F1B2976CD82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C76A581D-70D9-4324-B3C2-C549CBC3A500}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A7812BB-980B-4585-92C6-973734300155}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6255,4 +6270,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59E2A907-BC75-4262-BBD0-4F1B2976CD82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C76A581D-70D9-4324-B3C2-C549CBC3A500}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>